<commit_message>
Xử lý nghiệp vụ xong 80% chức năng đăng tin rao vặt Chỉnh sửa hyperlink của masterpage
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="OLE_LINK1" localSheetId="0">Sheet1!$B$8</definedName>
+    <definedName name="OLE_LINK1" localSheetId="0">Sheet1!$B$7</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>STT</t>
   </si>
@@ -42,9 +42,6 @@
     <t>XTiến</t>
   </si>
   <si>
-    <t>Hiển thị danh sách mục rao vặt con</t>
-  </si>
-  <si>
     <t>Thêm chức năng xem nội dung tin rao vặt.</t>
   </si>
   <si>
@@ -79,6 +76,27 @@
   </si>
   <si>
     <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>Xem tin nhắn của mình</t>
+  </si>
+  <si>
+    <t>Thuận</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Chưa có validator, chưa xử lý fileupload</t>
+  </si>
+  <si>
+    <t>Hiển thị danh sách mục rao vặt con (danh mục chính)</t>
+  </si>
+  <si>
+    <t>Hình ảnh chưa phù hợp</t>
+  </si>
+  <si>
+    <t>Hiển thị chưa logic lắm (cần hiển thị tên, không phải mã người dùng)</t>
   </si>
 </sst>
 </file>
@@ -142,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -154,6 +172,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,19 +475,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75">
@@ -480,7 +506,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -495,77 +521,79 @@
         <v>6</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="F3" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2">
@@ -576,10 +604,10 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2">
@@ -590,56 +618,66 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2">
+        <v>2.4</v>
+      </c>
       <c r="D10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2">
         <v>2.4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="45">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2">
-        <v>2.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2">
@@ -649,7 +687,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2">
@@ -659,7 +697,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2">
@@ -669,7 +707,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2">
@@ -679,17 +717,17 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2">
@@ -699,7 +737,7 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2">
@@ -709,7 +747,7 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2">
@@ -719,7 +757,7 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2">
@@ -729,7 +767,7 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2">
@@ -739,7 +777,7 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2">
@@ -749,7 +787,7 @@
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2">
@@ -759,17 +797,7 @@
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="2">
-        <v>24</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="F24" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
//Chỉnh sửa CSDL - Xóa bảng ChiTietTinRaoVatThuong - Bảng TinRaoVat: thêm cột GhiChu - Bảng DanhMucChinh: đổi thứ tự 3 danh mục ứng với 3 chuyên mục lên đầu (ở phần câu lệnh insert) - Bảng DanhMucCon: thêm dữ liệu và đổi lại tương ứng với DanhMucChinh //Bố cục lại trang chọn chuyên mục //Chỉnh lại màu sắc từng view đăng tin //Xử lý Fileupload (Thumbnail cho TinRaoVat)
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>STT</t>
   </si>
@@ -520,7 +520,9 @@
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6">
@@ -534,7 +536,9 @@
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F3" s="5" t="s">
         <v>24</v>
       </c>
@@ -550,7 +554,9 @@
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6">
@@ -564,7 +570,9 @@
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6">
@@ -578,7 +586,9 @@
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6">

</xml_diff>

<commit_message>
Thêm validator cho từng view đăng tin
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="OLE_LINK1" localSheetId="0">Sheet1!$B$7</definedName>
+    <definedName name="OLE_LINK1" localSheetId="0">Sheet1!$B$9</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>STT</t>
   </si>
@@ -87,9 +87,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>Chưa có validator, chưa xử lý fileupload</t>
-  </si>
-  <si>
     <t>Hiển thị danh sách mục rao vặt con (danh mục chính)</t>
   </si>
   <si>
@@ -97,6 +94,21 @@
   </si>
   <si>
     <t>Hiển thị chưa logic lắm (cần hiển thị tên, không phải mã người dùng)</t>
+  </si>
+  <si>
+    <t>Quên mật khẩu</t>
+  </si>
+  <si>
+    <t>Không có Rich text editor và FileUpload filter.</t>
+  </si>
+  <si>
+    <t>Thiết kế Masterpage</t>
+  </si>
+  <si>
+    <t>Thiết kế các User Control</t>
+  </si>
+  <si>
+    <t>Design đúng nhưng hiển thị bị lỗi</t>
   </si>
 </sst>
 </file>
@@ -162,24 +174,26 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -475,7 +489,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -486,328 +500,322 @@
     <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="30">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" ht="45">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="16" spans="1:6">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" ht="30">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="2">
-        <v>2.4</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="2">
-        <v>2.4</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" ht="45">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="C12" s="2">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="2">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="2">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="2">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="2">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="2">
-        <v>23</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Thiết kế giao diện cơ bản cho chức năng Chỉnh sửa tin rao vặt Commit tài liệu phân quyền (slide của cô và phim demo) Commit hai demo về hiển thị menu Gom 3 file demo vào thư mục Demo
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>STT</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>Design đúng nhưng hiển thị bị lỗi</t>
+  </si>
+  <si>
+    <t>Nhắn tin cho người dùng khác</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa bài rao vặt</t>
+  </si>
+  <si>
+    <t>Cần viết lớp riêng</t>
   </si>
 </sst>
 </file>
@@ -489,7 +498,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -646,7 +655,9 @@
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="D9" s="3" t="s">
         <v>14</v>
       </c>
@@ -662,14 +673,18 @@
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="D10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="3">
@@ -678,7 +693,9 @@
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="D11" s="3" t="s">
         <v>14</v>
       </c>
@@ -692,7 +709,9 @@
       <c r="B12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="3">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="D12" s="3" t="s">
         <v>14</v>
       </c>
@@ -726,54 +745,66 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C14" s="3">
         <v>2.4</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" ht="45">
+    <row r="15" spans="1:6">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C15" s="3">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>15</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" ht="45">
       <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="5"/>
+      <c r="B16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="B17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="E17" s="3"/>
       <c r="F17" s="5"/>
     </row>
@@ -801,11 +832,11 @@
       <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="3">
@@ -816,6 +847,16 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Chỉnh sửa MaDanhMucCon của các câu lệnh insert TinRaoVatThuong, ... Hiển thị giao diện chỉnh sửa cho 2 view đầu.
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>STT</t>
   </si>
@@ -42,9 +42,6 @@
     <t>XTiến</t>
   </si>
   <si>
-    <t>Thêm chức năng xem nội dung tin rao vặt.</t>
-  </si>
-  <si>
     <t>Xem thông tin liên hệ.</t>
   </si>
   <si>
@@ -118,6 +115,12 @@
   </si>
   <si>
     <t>Đang dùng phân quyển mặc định</t>
+  </si>
+  <si>
+    <t>Xem nội dung tin rao vặt.</t>
+  </si>
+  <si>
+    <t>Chỉ mới xem được tin rao vặt thường</t>
   </si>
 </sst>
 </file>
@@ -501,7 +504,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -531,7 +534,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -546,7 +549,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -555,17 +558,17 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -573,49 +576,51 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="30">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -623,14 +628,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="5"/>
     </row>
@@ -639,14 +644,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="5"/>
     </row>
@@ -655,16 +660,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3">
         <v>1.1000000000000001</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="5"/>
     </row>
@@ -673,19 +678,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3">
         <v>1.1000000000000001</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -693,13 +698,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3">
         <v>1.1000000000000001</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="5"/>
@@ -709,16 +714,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="3">
         <v>1.1000000000000001</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="5"/>
     </row>
@@ -727,19 +732,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="3">
         <v>2.4</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -747,13 +752,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="3">
         <v>2.4</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="5"/>
@@ -763,13 +768,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="3">
         <v>2.4</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="5"/>
@@ -779,19 +784,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="3">
         <v>2.2999999999999998</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -799,16 +804,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="3">
         <v>2.2999999999999998</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F17" s="5"/>
     </row>

</xml_diff>

<commit_message>
Thêm các file phân công Chỉnh sửa CSDL/WEBRAOVAT.sql - Chỉnh sửa các câu lệnh insert dữ liệu liên quan các loại  TinRaoVat Hoàn tất giao diện chức năng chỉnh sửa tin rao vặt
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -12,14 +12,15 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="OLE_LINK1" localSheetId="0">Sheet1!$B$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$F$24</definedName>
+    <definedName name="OLE_LINK1" localSheetId="0">Sheet1!$B$11</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
   <si>
     <t>STT</t>
   </si>
@@ -111,16 +112,46 @@
     <t>Chỉnh sửa bài rao vặt</t>
   </si>
   <si>
-    <t>Cần viết lớp riêng</t>
-  </si>
-  <si>
     <t>Đang dùng phân quyển mặc định</t>
   </si>
   <si>
     <t>Xem nội dung tin rao vặt.</t>
   </si>
   <si>
-    <t>Chỉ mới xem được tin rao vặt thường</t>
+    <t>Hoàn tất giao diện chỉnh sửa</t>
+  </si>
+  <si>
+    <t>Không xem được?</t>
+  </si>
+  <si>
+    <t>Tìm kiếm cơ bản</t>
+  </si>
+  <si>
+    <t>Tìm kiếm nâng cao</t>
+  </si>
+  <si>
+    <t>Đăng ký email để nhận tin rao vặt mới theo từng mục hay tất cả.</t>
+  </si>
+  <si>
+    <t>Xem và Chỉnh sửa thông tin cá nhân.</t>
+  </si>
+  <si>
+    <t>Báo cáo bài viết vi hoặc thành viên phạm nội quy</t>
+  </si>
+  <si>
+    <t>Chuyển đổi tài khoản lên VIP</t>
+  </si>
+  <si>
+    <t>Thanh toán trực tuyến phí chuyển đổi</t>
+  </si>
+  <si>
+    <t>Cần viết lớp riêng để xử lý</t>
+  </si>
+  <si>
+    <t>Đề nghị bỏ cột Photo, thêm cột Địa điểm</t>
+  </si>
+  <si>
+    <t>Cần thông báo đăng ký thành công</t>
   </si>
 </sst>
 </file>
@@ -184,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -199,12 +230,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -501,20 +526,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75">
@@ -542,7 +565,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
@@ -551,14 +574,16 @@
       <c r="E2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
@@ -567,34 +592,38 @@
       <c r="E3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="30">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.2</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" ht="30">
+      <c r="F4" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.2</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
@@ -602,7 +631,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -610,34 +639,38 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.2</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.2</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="3">
@@ -646,7 +679,9 @@
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3">
+        <v>1.2</v>
+      </c>
       <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
@@ -660,17 +695,15 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>20</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E9" s="3"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6">
@@ -678,27 +711,23 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="C10" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3">
         <v>1.1000000000000001</v>
@@ -706,15 +735,19 @@
       <c r="D11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="5"/>
+      <c r="E11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C12" s="3">
         <v>1.1000000000000001</v>
@@ -725,56 +758,58 @@
       <c r="E12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="30">
+      <c r="F12" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3">
-        <v>2.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C14" s="3">
-        <v>2.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="30">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C15" s="3">
-        <v>2.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="5"/>
@@ -784,66 +819,86 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C16" s="3">
-        <v>2.2999999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>13</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" ht="30">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C17" s="3">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="5"/>
+      <c r="F17" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="B18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="B19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="B20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20" s="5"/>
     </row>
@@ -851,23 +906,74 @@
       <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="7"/>
+      <c r="B21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="7"/>
+      <c r="B22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="5"/>
     </row>
   </sheetData>
+  <autoFilter ref="B1:F24"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Hoàn thành chức năng chỉnh sửa tin rao vặt (4 loại). Chỉnh sửa link ở MasterPage.master Chỉnh sửa gridview của trang default.aspx
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
   <si>
     <t>STT</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>Xem nội dung tin rao vặt.</t>
-  </si>
-  <si>
-    <t>Hoàn tất giao diện chỉnh sửa</t>
   </si>
   <si>
     <t>Không xem được?</t>
@@ -528,7 +525,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -540,7 +539,7 @@
     <col min="6" max="6" width="37.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75">
+    <row r="1" spans="1:6" ht="47.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -611,10 +610,10 @@
         <v>20</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -669,7 +668,7 @@
         <v>20</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -695,7 +694,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="3">
         <v>1.3</v>
@@ -711,7 +710,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="3">
         <v>1.3</v>
@@ -739,7 +738,7 @@
         <v>20</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -759,7 +758,7 @@
         <v>20</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -803,7 +802,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="3">
         <v>1.1000000000000001</v>
@@ -819,7 +818,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="3">
         <v>2.1</v>
@@ -850,7 +849,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" ht="30">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -863,9 +862,11 @@
       <c r="D18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F18" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -891,7 +892,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="3">
         <v>2.2000000000000002</v>
@@ -907,7 +908,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="3">
         <v>2.2000000000000002</v>
@@ -961,7 +962,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="3">
         <v>2.5</v>

</xml_diff>

<commit_message>
Cập nhật Danh sach chuc nang/Features.xlsx
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$F$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$F$26</definedName>
     <definedName name="OLE_LINK1" localSheetId="0">Sheet1!$B$11</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="89">
   <si>
     <t>STT</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Chỉnh sửa bài rao vặt</t>
   </si>
   <si>
-    <t>Đang dùng phân quyển mặc định</t>
-  </si>
-  <si>
     <t>Xem nội dung tin rao vặt.</t>
   </si>
   <si>
@@ -149,13 +146,157 @@
   </si>
   <si>
     <t>Cần thông báo đăng ký thành công</t>
+  </si>
+  <si>
+    <t>WEBSITE RAO VẶT</t>
+  </si>
+  <si>
+    <t>Chức năng</t>
+  </si>
+  <si>
+    <t>Điểm
+chuẩn</t>
+  </si>
+  <si>
+    <t>Mức độ
+hoàn thành</t>
+  </si>
+  <si>
+    <t>Điểm Giáo
+viên</t>
+  </si>
+  <si>
+    <t>1. Phân hệ Guest</t>
+  </si>
+  <si>
+    <t>- Đăng ký tài khoản thành viên thường (Member)</t>
+  </si>
+  <si>
+    <t>- Đăng ký email để nhận tin rao vặt mới theo từng mục hay tất cả.</t>
+  </si>
+  <si>
+    <t>Đăng nhập.</t>
+  </si>
+  <si>
+    <t>Xem thông tin rao vặt:</t>
+  </si>
+  <si>
+    <t>+ Xem danh sách tất cả các mục rao vặt chính</t>
+  </si>
+  <si>
+    <t>+ Xem danh sách các mục rao vặt con trong một mục chính</t>
+  </si>
+  <si>
+    <t>+ Xem danh sách các bài rao vặt theo nội dung</t>
+  </si>
+  <si>
+    <t>+ Xem danh nội dung bài rao vặt</t>
+  </si>
+  <si>
+    <t>+ Xem thông tin liên hệ người dùng</t>
+  </si>
+  <si>
+    <t>Tìm kiếm</t>
+  </si>
+  <si>
+    <t>- Tìm cơ bản</t>
+  </si>
+  <si>
+    <t>- Tìm nâng cao</t>
+  </si>
+  <si>
+    <t>Lựa chọn ngôn ngữ Anh - Việt</t>
+  </si>
+  <si>
+    <t>2. Phân hệ Member thường (có tất cả các chức năng của Guest)</t>
+  </si>
+  <si>
+    <t>Các chức năng tô màu đỏ là chức năng nâng cao cộng điểm</t>
+  </si>
+  <si>
+    <t>Thông tin cá nhân</t>
+  </si>
+  <si>
+    <t>- Xem và Chỉnh sửa thông tin cá nhân.</t>
+  </si>
+  <si>
+    <t>- Lấy lại mật khẩu.</t>
+  </si>
+  <si>
+    <t>Đăng Xuất.</t>
+  </si>
+  <si>
+    <t>- Thanh toán trực tuyến phí chuyển đổi</t>
+  </si>
+  <si>
+    <t>Quản lý Tin nhắn</t>
+  </si>
+  <si>
+    <t>- Xem tin nhắn của mình</t>
+  </si>
+  <si>
+    <t>- Nhắn tin cho người dùng khác</t>
+  </si>
+  <si>
+    <t>Quản lý bài rao vặt</t>
+  </si>
+  <si>
+    <t>- Đăng bài rao vặt ở mục bất kỳ và các chuyên mục đặc biệt (bất động sản, việc làm)</t>
+  </si>
+  <si>
+    <t>- Chỉnh sửa bài rao vặt hoặc trả lời của mình</t>
+  </si>
+  <si>
+    <t>- Trả lời cho bài rao vặt của mình hoặc của người khác</t>
+  </si>
+  <si>
+    <t>3. Phân hệ Member VIP (có tất cả các chức năng của Member thường)</t>
+  </si>
+  <si>
+    <t>Up bài tự động theo thời gian người dùng tự quy định</t>
+  </si>
+  <si>
+    <t>Đăng bài viết lên phần nổi bật</t>
+  </si>
+  <si>
+    <t>Phát tán tin rao vặt</t>
+  </si>
+  <si>
+    <t>4. Phân hệ Admin (có giao diện template riêng khác với các phân hệ khác)</t>
+  </si>
+  <si>
+    <t>Quản lý tin rao vặt</t>
+  </si>
+  <si>
+    <t>- Xem và duyệt tin rao vặt</t>
+  </si>
+  <si>
+    <t>- Thêm, Xóa tin rao vặt</t>
+  </si>
+  <si>
+    <t>Quản lý chuyên mục chính, chuyên mục con</t>
+  </si>
+  <si>
+    <t>- Thêm, Xóa, Sửa</t>
+  </si>
+  <si>
+    <t>Quản lý tài khoản</t>
+  </si>
+  <si>
+    <t>Quản lý Banner/ logo/ theme</t>
+  </si>
+  <si>
+    <t>Đang dùng phân quyền mặc định</t>
+  </si>
+  <si>
+    <t>Gửi email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,16 +317,68 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -208,11 +401,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -228,6 +473,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -610,7 +888,7 @@
         <v>20</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30">
@@ -656,7 +934,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="3">
         <v>1.2</v>
@@ -668,7 +946,7 @@
         <v>20</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -694,7 +972,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="3">
         <v>1.3</v>
@@ -702,7 +980,9 @@
       <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6">
@@ -710,7 +990,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="3">
         <v>1.3</v>
@@ -738,7 +1018,7 @@
         <v>20</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -758,7 +1038,7 @@
         <v>20</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -802,7 +1082,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="3">
         <v>1.1000000000000001</v>
@@ -818,7 +1098,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="3">
         <v>2.1</v>
@@ -874,17 +1154,15 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="C19" s="3">
-        <v>2.4</v>
+        <v>1.4</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>20</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E19" s="3"/>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6">
@@ -892,13 +1170,11 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="3">
-        <v>2.2000000000000002</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="5"/>
@@ -908,15 +1184,17 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="C21" s="3">
-        <v>2.2000000000000002</v>
+        <v>2.4</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6">
@@ -924,37 +1202,31 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C22" s="3">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C23" s="3">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E23" s="3"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6">
@@ -962,19 +1234,61 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C24" s="3">
-        <v>2.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="5"/>
+      <c r="E24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:F24"/>
+  <autoFilter ref="B1:F26"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -982,13 +1296,571 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="75.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" ht="30">
+      <c r="A3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="18"/>
+      <c r="B6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="18"/>
+      <c r="B7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="18"/>
+      <c r="B8" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="18">
+        <v>1.2</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="18">
+        <v>1</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="18"/>
+      <c r="B10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="18"/>
+      <c r="B11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="18"/>
+      <c r="B12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="18"/>
+      <c r="B13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="18"/>
+      <c r="B14" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="18">
+        <v>1.3</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="18">
+        <v>1</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="18"/>
+      <c r="B16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="18"/>
+      <c r="B17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="10">
+        <v>1.4</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="18">
+        <v>2.1</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="18"/>
+      <c r="B21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="18"/>
+      <c r="B22" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="18"/>
+      <c r="B23" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="18">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="18"/>
+      <c r="B25" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="18">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="18"/>
+      <c r="B27" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="18"/>
+      <c r="B28" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="18">
+        <v>2.4</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="18"/>
+      <c r="B30" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="18"/>
+      <c r="B31" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="18"/>
+      <c r="B32" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="10">
+        <v>3.1</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="10">
+        <v>3.2</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="18">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="18"/>
+      <c r="B40" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="18"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="18"/>
+      <c r="B41" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="18"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="18">
+        <v>4.2</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="18">
+        <v>1</v>
+      </c>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="18"/>
+      <c r="B43" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="18"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="18">
+        <v>4.3</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="18"/>
+      <c r="B45" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" s="18"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="18">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="18"/>
+      <c r="B47" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="18"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="49">
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Phân công tuần (6/6 - 11/6): các anh em theo phân công mà làm nha: Trong 2 file: Features.xlsx và file CheckList DoAn_RaoVat.pdf
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -12,15 +12,15 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$F$26</definedName>
-    <definedName name="OLE_LINK1" localSheetId="0">Sheet1!$B$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$F$29</definedName>
+    <definedName name="OLE_LINK1" localSheetId="0">Sheet1!$B$12</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="95">
   <si>
     <t>STT</t>
   </si>
@@ -290,13 +290,33 @@
   </si>
   <si>
     <t>Gửi email</t>
+  </si>
+  <si>
+    <t>Tiếp tục</t>
+  </si>
+  <si>
+    <t>Mới</t>
+  </si>
+  <si>
+    <t>Quản lý chuyên mục chính, chuyên mục con: Thêm, Xóa, Sửa</t>
+  </si>
+  <si>
+    <t>X.Tiến</t>
+  </si>
+  <si>
+    <t>Quản lý tài khoản: Thêm, Xóa, Sửa</t>
+  </si>
+  <si>
+    <t>Quản lý tin rao vặt:
+Xem và duyệt tin rao vặt
+Thêm, Xóa tin rao vặt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,8 +377,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,8 +410,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -453,26 +516,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -489,6 +556,15 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -498,14 +574,126 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -801,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B30" sqref="B30:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -837,458 +1025,544 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="3">
+    <row r="2" spans="1:6" ht="15.75">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3">
+    <row r="3" spans="1:6" ht="15.75">
+      <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="18"/>
+      <c r="D3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="1:6" ht="30">
-      <c r="A4" s="3">
+      <c r="A4" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="18">
         <v>1.2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="20" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30">
-      <c r="A5" s="3">
+      <c r="A5" s="18">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="18">
         <v>1.2</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3">
+    <row r="6" spans="1:6" ht="15.75">
+      <c r="A6" s="18">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="18">
         <v>1.2</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="3">
+      <c r="F6" s="20"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75">
+      <c r="A7" s="18">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="18">
         <v>1.2</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="3">
+    <row r="8" spans="1:6" ht="15.75">
+      <c r="A8" s="18">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="18">
         <v>1.2</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="3">
+      <c r="F8" s="20"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75">
+      <c r="A9" s="18">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="18">
         <v>1.3</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="3">
+      <c r="F9" s="20"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75">
+      <c r="A10" s="18">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="18">
         <v>1.3</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="3">
+      <c r="E10" s="18"/>
+      <c r="F10" s="58" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="31.5">
+      <c r="A11" s="36">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="51">
+        <v>4.2</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="51"/>
+      <c r="F11" s="52" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="18">
+        <v>12</v>
+      </c>
+      <c r="B12" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C12" s="24">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E12" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F12" s="26" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="3">
+    <row r="13" spans="1:6">
+      <c r="A13" s="18">
+        <v>13</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="18">
+        <v>14</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="26"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="18">
+        <v>15</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="26"/>
+    </row>
+    <row r="16" spans="1:6" ht="30">
+      <c r="A16" s="18">
+        <v>16</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="24"/>
+      <c r="F16" s="57" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="18">
+        <v>17</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="24">
+        <v>2.1</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="24"/>
+      <c r="F17" s="57" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75">
+      <c r="A18" s="36">
+        <v>18</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="48">
+        <v>4.3</v>
+      </c>
+      <c r="D18" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="48"/>
+      <c r="F18" s="49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30">
+      <c r="A19" s="18">
+        <v>20</v>
+      </c>
+      <c r="B19" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="C19" s="27">
+        <v>2.4</v>
+      </c>
+      <c r="D19" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="3">
+      <c r="F19" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30">
+      <c r="A20" s="18">
+        <v>21</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="27">
+        <v>2.4</v>
+      </c>
+      <c r="D20" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="E20" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="F20" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75">
+      <c r="A21" s="36">
+        <v>22</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="45">
+        <v>1.4</v>
+      </c>
+      <c r="D21" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="45"/>
+      <c r="F21" s="46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75">
+      <c r="A22" s="36">
         <v>23</v>
       </c>
-      <c r="C14" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="B22" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="45"/>
+      <c r="F22" s="46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="18">
+        <v>25</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="21">
+        <v>2.4</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" ht="30">
-      <c r="A15" s="3">
+      <c r="F23" s="23"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="18">
+        <v>26</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="21">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D24" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" ht="30">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="E24" s="21"/>
+      <c r="F24" s="56" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="18">
+        <v>27</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="21">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="21"/>
+      <c r="F25" s="56" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75">
+      <c r="A26" s="36">
+        <v>28</v>
+      </c>
+      <c r="B26" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="42">
+        <v>3.2</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="42"/>
+      <c r="F26" s="43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75">
+      <c r="A27" s="18">
+        <v>30</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="30">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D27" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="F27" s="32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75">
+      <c r="A28" s="18">
+        <v>31</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="30">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D28" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="3">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="3">
+      <c r="F28" s="32"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75">
+      <c r="A29" s="18">
+        <v>32</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="33">
+        <v>2.5</v>
+      </c>
+      <c r="D29" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="3">
+      <c r="E29" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="3">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="3">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="3">
-        <v>23</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="F29" s="35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="47.25">
+      <c r="A30" s="36">
+        <v>33</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="38">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D30" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="3">
-        <v>24</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="3">
-        <v>25</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>87</v>
+      <c r="E30" s="39"/>
+      <c r="F30" s="40" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:F26"/>
+  <autoFilter ref="B1:F29"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1311,504 +1585,537 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="11" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="18">
+      <c r="A5" s="14">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="14">
         <v>0.75</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="18"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="18"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="18"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="18"/>
+      <c r="C7" s="14"/>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="18"/>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="18">
+      <c r="A9" s="14">
         <v>1.2</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="14">
         <v>1</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="18"/>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="14"/>
+      <c r="B10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="18"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="18"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="18"/>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="14"/>
+      <c r="B12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="18"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="18"/>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="18"/>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="14"/>
+      <c r="B14" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="18">
+      <c r="A15" s="14">
         <v>1.3</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="14">
         <v>1</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="18"/>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="14"/>
+      <c r="B16" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="18"/>
+      <c r="C16" s="14"/>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="18"/>
-      <c r="B17" s="7" t="s">
+      <c r="A17" s="14"/>
+      <c r="B17" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="18"/>
+      <c r="C17" s="14"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="10">
+      <c r="A18" s="7">
         <v>1.4</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="7">
         <v>0.5</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="18">
+      <c r="A20" s="14">
         <v>2.1</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="14">
         <v>0.75</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="18"/>
-      <c r="B21" s="7" t="s">
+      <c r="A21" s="14"/>
+      <c r="B21" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="18"/>
+      <c r="C21" s="14"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="18"/>
-      <c r="B22" s="7" t="s">
+      <c r="A22" s="14"/>
+      <c r="B22" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="18"/>
+      <c r="C22" s="14"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="18"/>
-      <c r="B23" s="9" t="s">
+      <c r="A23" s="14"/>
+      <c r="B23" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="18"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="18">
+      <c r="A24" s="14">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="14">
         <v>0.5</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="18"/>
-      <c r="B25" s="7" t="s">
+      <c r="A25" s="14"/>
+      <c r="B25" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="18"/>
+      <c r="C25" s="14"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="18">
+      <c r="A26" s="14">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="14">
         <v>0.75</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="18"/>
-      <c r="B27" s="7" t="s">
+      <c r="A27" s="14"/>
+      <c r="B27" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="18"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="18"/>
-      <c r="B28" s="7" t="s">
+      <c r="A28" s="14"/>
+      <c r="B28" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="18"/>
+      <c r="C28" s="14"/>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="18">
+      <c r="A29" s="14">
         <v>2.4</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="18">
+      <c r="C29" s="14">
         <v>1.5</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="18"/>
-      <c r="B30" s="7" t="s">
+      <c r="A30" s="14"/>
+      <c r="B30" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="18"/>
+      <c r="C30" s="14"/>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="18"/>
-      <c r="B31" s="7" t="s">
+      <c r="A31" s="14"/>
+      <c r="B31" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="18"/>
+      <c r="C31" s="14"/>
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="18"/>
-      <c r="B32" s="7" t="s">
+      <c r="A32" s="14"/>
+      <c r="B32" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="18"/>
+      <c r="C32" s="14"/>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="10">
+      <c r="A33" s="7">
         <v>2.5</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="7">
         <v>0.5</v>
       </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="10">
+      <c r="A35" s="7">
         <v>3.1</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="7">
         <v>0.5</v>
       </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="10">
+      <c r="A36" s="7">
         <v>3.2</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="7">
         <v>0.5</v>
       </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="10">
+      <c r="A37" s="7">
         <v>3.3</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="7">
         <v>0.5</v>
       </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="18">
+      <c r="A39" s="14">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="18">
+      <c r="C39" s="14">
         <v>0.5</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="15"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="18"/>
-      <c r="B40" s="7" t="s">
+      <c r="A40" s="14"/>
+      <c r="B40" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C40" s="18"/>
+      <c r="C40" s="14"/>
       <c r="D40" s="17"/>
       <c r="E40" s="17"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="18"/>
-      <c r="B41" s="7" t="s">
+      <c r="A41" s="14"/>
+      <c r="B41" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C41" s="18"/>
+      <c r="C41" s="14"/>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="18">
+      <c r="A42" s="14">
         <v>4.2</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="18">
+      <c r="C42" s="14">
         <v>1</v>
       </c>
       <c r="D42" s="15"/>
       <c r="E42" s="15"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="18"/>
-      <c r="B43" s="7" t="s">
+      <c r="A43" s="14"/>
+      <c r="B43" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="18"/>
+      <c r="C43" s="14"/>
       <c r="D43" s="16"/>
       <c r="E43" s="16"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="18">
+      <c r="A44" s="14">
         <v>4.3</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C44" s="18">
+      <c r="C44" s="14">
         <v>0.5</v>
       </c>
       <c r="D44" s="15"/>
       <c r="E44" s="15"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="18"/>
-      <c r="B45" s="7" t="s">
+      <c r="A45" s="14"/>
+      <c r="B45" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C45" s="18"/>
+      <c r="C45" s="14"/>
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="18">
+      <c r="A46" s="14">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C46" s="18">
+      <c r="C46" s="14">
         <v>0.75</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="15"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="18"/>
-      <c r="B47" s="7" t="s">
+      <c r="A47" s="14"/>
+      <c r="B47" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="18"/>
+      <c r="C47" s="14"/>
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A44:A45"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A20:A23"/>
@@ -1825,39 +2132,6 @@
     <mergeCell ref="C9:C14"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="A26:A28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D5:D8"/>
-    <mergeCell ref="E5:E8"/>
-    <mergeCell ref="D9:D14"/>
-    <mergeCell ref="E9:E14"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cập nhật lại các chức năng làm được.
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="96">
   <si>
     <t>STT</t>
   </si>
@@ -139,13 +139,7 @@
     <t>Thanh toán trực tuyến phí chuyển đổi</t>
   </si>
   <si>
-    <t>Cần viết lớp riêng để xử lý</t>
-  </si>
-  <si>
     <t>Đề nghị bỏ cột Photo, thêm cột Địa điểm</t>
-  </si>
-  <si>
-    <t>Cần thông báo đăng ký thành công</t>
   </si>
   <si>
     <t>WEBSITE RAO VẶT</t>
@@ -310,13 +304,22 @@
     <t>Quản lý tin rao vặt:
 Xem và duyệt tin rao vặt
 Thêm, Xóa tin rao vặt</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>OK, chỉ mới xem được</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,6 +390,11 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFFFF00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -556,24 +564,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -689,10 +679,28 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -991,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1026,539 +1034,539 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75">
-      <c r="A2" s="18">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="36" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75">
-      <c r="A3" s="18">
+      <c r="A3" s="12">
         <v>2</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="36" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="20"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:6" ht="30">
-      <c r="A4" s="18">
+      <c r="A4" s="12">
         <v>3</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="12">
         <v>1.2</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="20" t="s">
-        <v>40</v>
+      <c r="F4" s="14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30">
-      <c r="A5" s="18">
+      <c r="A5" s="12">
         <v>4</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="12">
         <v>1.2</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75">
-      <c r="A6" s="18">
+      <c r="A6" s="12">
         <v>5</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="12">
         <v>1.2</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="20"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" ht="15.75">
-      <c r="A7" s="18">
+      <c r="A7" s="12">
         <v>6</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="12">
         <v>1.2</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75">
-      <c r="A8" s="18">
+      <c r="A8" s="12">
         <v>7</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="12">
         <v>1.2</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="20"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" ht="15.75">
-      <c r="A9" s="18">
+      <c r="A9" s="12">
         <v>8</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="12">
         <v>1.3</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="20"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="15.75">
-      <c r="A10" s="18">
+      <c r="A10" s="12">
         <v>9</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="12">
         <v>1.3</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="58" t="s">
+      <c r="E10" s="12"/>
+      <c r="F10" s="51" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="31.5">
+      <c r="A11" s="30">
+        <v>10</v>
+      </c>
+      <c r="B11" s="44" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="31.5">
-      <c r="A11" s="36">
+      <c r="C11" s="45">
+        <v>4.2</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="45"/>
+      <c r="F11" s="46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="12">
+        <v>13</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="12">
+        <v>14</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="C14" s="18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="20"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="12">
+        <v>15</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="20"/>
+    </row>
+    <row r="16" spans="1:6" ht="30">
+      <c r="A16" s="12">
+        <v>16</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="58" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="12">
+        <v>17</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="18">
+        <v>2.1</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="58" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75">
+      <c r="A18" s="30">
+        <v>18</v>
+      </c>
+      <c r="B18" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="51">
-        <v>4.2</v>
-      </c>
-      <c r="D11" s="51" t="s">
+      <c r="C18" s="42">
+        <v>4.3</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="42"/>
+      <c r="F18" s="43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30">
+      <c r="A19" s="12">
+        <v>20</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="21">
+        <v>2.4</v>
+      </c>
+      <c r="D19" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30">
+      <c r="A20" s="12">
+        <v>21</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="21">
+        <v>2.4</v>
+      </c>
+      <c r="D20" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75">
+      <c r="A21" s="30">
+        <v>22</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="39">
+        <v>1.4</v>
+      </c>
+      <c r="D21" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="39"/>
+      <c r="F21" s="40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75">
+      <c r="A22" s="30">
+        <v>23</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="39"/>
+      <c r="F22" s="40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="12">
+        <v>25</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="15">
+        <v>2.4</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="17"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="12">
+        <v>26</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="15"/>
+      <c r="F24" s="50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="12">
+        <v>27</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="15"/>
+      <c r="F25" s="50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75">
+      <c r="A26" s="30">
+        <v>28</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="36">
+        <v>3.2</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="36"/>
+      <c r="F26" s="37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75">
+      <c r="A27" s="12">
+        <v>30</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="24">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D27" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75">
+      <c r="A28" s="12">
+        <v>31</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="24">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D28" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="26"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75">
+      <c r="A29" s="12">
+        <v>32</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="27">
+        <v>2.5</v>
+      </c>
+      <c r="D29" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="47.25">
+      <c r="A30" s="30">
+        <v>33</v>
+      </c>
+      <c r="B30" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="E11" s="51"/>
-      <c r="F11" s="52" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="18">
-        <v>12</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="24">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="18">
-        <v>13</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="24">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="18">
-        <v>14</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="24">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="26"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="18">
-        <v>15</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="24">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="26"/>
-    </row>
-    <row r="16" spans="1:6" ht="30">
-      <c r="A16" s="18">
-        <v>16</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="24">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="57" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="18">
-        <v>17</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="24">
-        <v>2.1</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="57" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75">
-      <c r="A18" s="36">
-        <v>18</v>
-      </c>
-      <c r="B18" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="C18" s="48">
-        <v>4.3</v>
-      </c>
-      <c r="D18" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="48"/>
-      <c r="F18" s="49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30">
-      <c r="A19" s="18">
-        <v>20</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="27">
-        <v>2.4</v>
-      </c>
-      <c r="D19" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30">
-      <c r="A20" s="18">
-        <v>21</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="27">
-        <v>2.4</v>
-      </c>
-      <c r="D20" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75">
-      <c r="A21" s="36">
-        <v>22</v>
-      </c>
-      <c r="B21" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="45">
-        <v>1.4</v>
-      </c>
-      <c r="D21" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="45"/>
-      <c r="F21" s="46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75">
-      <c r="A22" s="36">
-        <v>23</v>
-      </c>
-      <c r="B22" s="44" t="s">
+      <c r="C30" s="32">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="33"/>
+      <c r="F30" s="34" t="s">
         <v>88</v>
-      </c>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="45"/>
-      <c r="F22" s="46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="18">
-        <v>25</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="21">
-        <v>2.4</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="23"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="18">
-        <v>26</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="21">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="56" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="18">
-        <v>27</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="21">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="56" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75">
-      <c r="A26" s="36">
-        <v>28</v>
-      </c>
-      <c r="B26" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" s="42">
-        <v>3.2</v>
-      </c>
-      <c r="D26" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="42"/>
-      <c r="F26" s="43" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75">
-      <c r="A27" s="18">
-        <v>30</v>
-      </c>
-      <c r="B27" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="30">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D27" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="32" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75">
-      <c r="A28" s="18">
-        <v>31</v>
-      </c>
-      <c r="B28" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="30">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D28" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="32"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75">
-      <c r="A29" s="18">
-        <v>32</v>
-      </c>
-      <c r="B29" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="33">
-        <v>2.5</v>
-      </c>
-      <c r="D29" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="35" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="47.25">
-      <c r="A30" s="36">
-        <v>33</v>
-      </c>
-      <c r="B30" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="38">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D30" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" s="39"/>
-      <c r="F30" s="40" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1585,20 +1593,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="A1" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1609,162 +1617,162 @@
         <v>0</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="11" t="s">
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="14">
+      <c r="A5" s="53">
         <v>1.1000000000000001</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="53">
         <v>0.75</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="14"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="53"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="53"/>
+      <c r="B7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="53"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="53"/>
+      <c r="B8" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="14"/>
-      <c r="B7" s="4" t="s">
+      <c r="C8" s="53"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="53">
+        <v>1.2</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="14"/>
-      <c r="B8" s="6" t="s">
+      <c r="C9" s="53">
+        <v>1</v>
+      </c>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="53"/>
+      <c r="B10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="14">
-        <v>1.2</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="C10" s="53"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="53"/>
+      <c r="B11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C11" s="53"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="53"/>
+      <c r="B12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="53"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="53"/>
+      <c r="B13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="53"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="53"/>
+      <c r="B14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="53"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="53">
+        <v>1.3</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="53">
         <v>1</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="14"/>
-      <c r="B10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="14"/>
-      <c r="B11" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="14"/>
-      <c r="B12" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="14"/>
-      <c r="B13" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="14"/>
-      <c r="B14" s="4" t="s">
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="53"/>
+      <c r="B16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="14">
-        <v>1.3</v>
-      </c>
-      <c r="B15" s="6" t="s">
+      <c r="C16" s="53"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="53"/>
+      <c r="B17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="14">
-        <v>1</v>
-      </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="14"/>
-      <c r="B16" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="14"/>
-      <c r="B17" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="7">
         <v>1.4</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C18" s="7">
         <v>0.5</v>
@@ -1773,146 +1781,146 @@
       <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="53">
+        <v>2.1</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="14">
-        <v>2.1</v>
-      </c>
-      <c r="B20" s="6" t="s">
+      <c r="C20" s="53">
+        <v>0.75</v>
+      </c>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="53"/>
+      <c r="B21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="53"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="53"/>
+      <c r="B22" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="14">
-        <v>0.75</v>
-      </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="14"/>
-      <c r="B21" s="4" t="s">
+      <c r="C22" s="53"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="53"/>
+      <c r="B23" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="14"/>
-      <c r="B22" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="14"/>
-      <c r="B23" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="14">
+      <c r="A24" s="53">
         <v>2.2000000000000002</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="53">
         <v>0.5</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="14"/>
+      <c r="A25" s="53"/>
       <c r="B25" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="53"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="53">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="53">
+        <v>0.75</v>
+      </c>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="53"/>
+      <c r="B27" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="14">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="C27" s="53"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="53"/>
+      <c r="B28" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="14">
-        <v>0.75</v>
-      </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="14"/>
-      <c r="B27" s="4" t="s">
+      <c r="C28" s="53"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="53">
+        <v>2.4</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="14"/>
-      <c r="B28" s="4" t="s">
+      <c r="C29" s="53">
+        <v>1.5</v>
+      </c>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="53"/>
+      <c r="B30" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="14">
-        <v>2.4</v>
-      </c>
-      <c r="B29" s="3" t="s">
+      <c r="C30" s="53"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="53"/>
+      <c r="B31" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="14"/>
-      <c r="B30" s="4" t="s">
+      <c r="C31" s="53"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="53"/>
+      <c r="B32" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="14"/>
-      <c r="B31" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="14"/>
-      <c r="B32" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="7">
@@ -1928,20 +1936,20 @@
       <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
+      <c r="A34" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="56"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="7">
         <v>3.1</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C35" s="7">
         <v>0.5</v>
@@ -1954,7 +1962,7 @@
         <v>3.2</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C36" s="7">
         <v>0.5</v>
@@ -1967,7 +1975,7 @@
         <v>3.3</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C37" s="7">
         <v>0.5</v>
@@ -1976,125 +1984,134 @@
       <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="56"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="53">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="53"/>
+      <c r="B40" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="14">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B39" s="6" t="s">
+      <c r="C40" s="53"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="53"/>
+      <c r="B41" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="14">
+      <c r="C41" s="53"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="53">
+        <v>4.2</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="53">
+        <v>1</v>
+      </c>
+      <c r="D42" s="54"/>
+      <c r="E42" s="54"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="53"/>
+      <c r="B43" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="53"/>
+      <c r="D43" s="55"/>
+      <c r="E43" s="55"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="53">
+        <v>4.3</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="53">
         <v>0.5</v>
       </c>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="14"/>
-      <c r="B40" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="14"/>
-      <c r="B41" s="4" t="s">
+      <c r="D44" s="54"/>
+      <c r="E44" s="54"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="53"/>
+      <c r="B45" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="14">
-        <v>4.2</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" s="14">
-        <v>1</v>
-      </c>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="14"/>
-      <c r="B43" s="4" t="s">
+      <c r="C45" s="53"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="53">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="14">
-        <v>4.3</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="14"/>
-      <c r="B45" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="14">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C46" s="14">
+      <c r="C46" s="53">
         <v>0.75</v>
       </c>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="54"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="14"/>
+      <c r="A47" s="53"/>
       <c r="B47" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
+        <v>82</v>
+      </c>
+      <c r="C47" s="53"/>
+      <c r="D47" s="55"/>
+      <c r="E47" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
     <mergeCell ref="D20:D23"/>
     <mergeCell ref="E20:E23"/>
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="D26:D28"/>
     <mergeCell ref="E26:E28"/>
-    <mergeCell ref="D5:D8"/>
-    <mergeCell ref="E5:E8"/>
-    <mergeCell ref="D9:D14"/>
-    <mergeCell ref="E9:E14"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A4:E4"/>
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="A38:E38"/>
     <mergeCell ref="A34:E34"/>
@@ -2107,16 +2124,6 @@
     <mergeCell ref="E29:E32"/>
     <mergeCell ref="D42:D43"/>
     <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A4:E4"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="A39:A41"/>
@@ -2132,6 +2139,7 @@
     <mergeCell ref="C9:C14"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="A26:A28"/>
+    <mergeCell ref="C29:C32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Sửa lỗi chức năng XemNoiDungTin.ascx Chỉnh lại giao diện phần trả lời trong XemNoiDungTin.ascx Chỉnh lại giao diện trang Default.aspx phần bên trái Cập nhật Features.xlsx
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -321,7 +321,7 @@
     <t>Cần tạo địa chỉ gmail chung cho nhóm.</t>
   </si>
   <si>
-    <t>Không làm được với MasterPage.</t>
+    <t>Không làm được với MasterPage và web user control</t>
   </si>
 </sst>
 </file>
@@ -691,32 +691,32 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1015,7 +1015,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1025,7 +1025,7 @@
     <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="47.25">
@@ -1388,36 +1388,36 @@
       <c r="A20" s="12">
         <v>21</v>
       </c>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="57">
+      <c r="C20" s="51">
         <v>2.4</v>
       </c>
-      <c r="D20" s="58" t="s">
+      <c r="D20" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="57" t="s">
+      <c r="E20" s="51" t="s">
         <v>20</v>
       </c>
       <c r="F20" s="23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75">
+    <row r="21" spans="1:6" ht="30">
       <c r="A21" s="30">
         <v>22</v>
       </c>
-      <c r="B21" s="56" t="s">
+      <c r="B21" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="57">
+      <c r="C21" s="51">
         <v>1.4</v>
       </c>
-      <c r="D21" s="58" t="s">
+      <c r="D21" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="58" t="s">
+      <c r="E21" s="52" t="s">
         <v>20</v>
       </c>
       <c r="F21" s="23" t="s">
@@ -1428,14 +1428,14 @@
       <c r="A22" s="30">
         <v>23</v>
       </c>
-      <c r="B22" s="56" t="s">
+      <c r="B22" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="C22" s="57"/>
-      <c r="D22" s="58" t="s">
+      <c r="C22" s="51"/>
+      <c r="D22" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="58" t="s">
+      <c r="E22" s="52" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="23" t="s">
@@ -1614,13 +1614,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
@@ -1651,142 +1651,142 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="51">
+      <c r="A5" s="55">
         <v>1.1000000000000001</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="51">
+      <c r="C5" s="55">
         <v>0.75</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="51"/>
+      <c r="A6" s="55"/>
       <c r="B6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="51"/>
+      <c r="A7" s="55"/>
       <c r="B7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="51"/>
+      <c r="A8" s="55"/>
       <c r="B8" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="51">
+      <c r="A9" s="55">
         <v>1.2</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="51">
+      <c r="C9" s="55">
         <v>1</v>
       </c>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="51"/>
+      <c r="A10" s="55"/>
       <c r="B10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="51"/>
+      <c r="A11" s="55"/>
       <c r="B11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="51"/>
+      <c r="A12" s="55"/>
       <c r="B12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="51"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="51"/>
+      <c r="A13" s="55"/>
       <c r="B13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="51"/>
+      <c r="A14" s="55"/>
       <c r="B14" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="51">
+      <c r="A15" s="55">
         <v>1.3</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="51">
+      <c r="C15" s="55">
         <v>1</v>
       </c>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="51"/>
+      <c r="A16" s="55"/>
       <c r="B16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="51"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="51"/>
+      <c r="A17" s="55"/>
       <c r="B17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="7">
@@ -1802,146 +1802,146 @@
       <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="51">
+      <c r="A20" s="55">
         <v>2.1</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="51">
+      <c r="C20" s="55">
         <v>0.75</v>
       </c>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="51"/>
+      <c r="A21" s="55"/>
       <c r="B21" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="51"/>
+      <c r="A22" s="55"/>
       <c r="B22" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="51"/>
+      <c r="A23" s="55"/>
       <c r="B23" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="51">
+      <c r="A24" s="55">
         <v>2.2000000000000002</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="51">
+      <c r="C24" s="55">
         <v>0.5</v>
       </c>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="51"/>
+      <c r="A25" s="55"/>
       <c r="B25" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="51"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="51">
+      <c r="A26" s="55">
         <v>2.2999999999999998</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="51">
+      <c r="C26" s="55">
         <v>0.75</v>
       </c>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="51"/>
+      <c r="A27" s="55"/>
       <c r="B27" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="51"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="51"/>
+      <c r="A28" s="55"/>
       <c r="B28" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="51"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="51">
+      <c r="A29" s="55">
         <v>2.4</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="51">
+      <c r="C29" s="55">
         <v>1.5</v>
       </c>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="51"/>
+      <c r="A30" s="55"/>
       <c r="B30" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="51"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="51"/>
+      <c r="A31" s="55"/>
       <c r="B31" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="51"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="51"/>
+      <c r="A32" s="55"/>
       <c r="B32" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="51"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="7">
@@ -1957,13 +1957,13 @@
       <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="54" t="s">
+      <c r="A34" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="54"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="7">
@@ -2005,130 +2005,129 @@
       <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="54" t="s">
+      <c r="A38" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="54"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="54"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="51">
+      <c r="A39" s="55">
         <v>4.0999999999999996</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C39" s="51">
+      <c r="C39" s="55">
         <v>0.5</v>
       </c>
-      <c r="D39" s="52"/>
-      <c r="E39" s="52"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="51"/>
+      <c r="A40" s="55"/>
       <c r="B40" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="51"/>
-      <c r="D40" s="55"/>
-      <c r="E40" s="55"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="51"/>
+      <c r="A41" s="55"/>
       <c r="B41" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="51"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="53"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="51">
+      <c r="A42" s="55">
         <v>4.2</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C42" s="51">
+      <c r="C42" s="55">
         <v>1</v>
       </c>
-      <c r="D42" s="52"/>
-      <c r="E42" s="52"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="51"/>
+      <c r="A43" s="55"/>
       <c r="B43" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="51"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="53"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="54"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="51">
+      <c r="A44" s="55">
         <v>4.3</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="51">
+      <c r="C44" s="55">
         <v>0.5</v>
       </c>
-      <c r="D44" s="52"/>
-      <c r="E44" s="52"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="51"/>
+      <c r="A45" s="55"/>
       <c r="B45" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C45" s="51"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="54"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="51">
+      <c r="A46" s="55">
         <v>4.4000000000000004</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C46" s="51">
+      <c r="C46" s="55">
         <v>0.75</v>
       </c>
-      <c r="D46" s="52"/>
-      <c r="E46" s="52"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="53"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="51"/>
+      <c r="A47" s="55"/>
       <c r="B47" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C47" s="51"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="53"/>
+      <c r="C47" s="55"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="D5:D8"/>
-    <mergeCell ref="E5:E8"/>
-    <mergeCell ref="D9:D14"/>
-    <mergeCell ref="E9:E14"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="C29:C32"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A46:A47"/>
@@ -2145,22 +2144,23 @@
     <mergeCell ref="E42:E43"/>
     <mergeCell ref="D20:D23"/>
     <mergeCell ref="E20:E23"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C42:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Chọn ngôn ngữ cho Master Page. Cập nhật file dll của Captcha. Cập nhật Features.xlsx.
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Phân công" sheetId="1" r:id="rId1"/>
@@ -320,7 +320,7 @@
     <t>Cần tạo địa chỉ gmail chung cho nhóm.</t>
   </si>
   <si>
-    <t>Không làm được với MasterPage và web user control</t>
+    <t>Chưa làm được với web user control</t>
   </si>
 </sst>
 </file>
@@ -700,23 +700,23 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1014,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1404,7 +1404,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30">
+    <row r="21" spans="1:6" ht="15.75">
       <c r="A21" s="30">
         <v>22</v>
       </c>
@@ -1601,7 +1601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
@@ -1614,13 +1614,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
@@ -1651,148 +1651,148 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="56">
+      <c r="A5" s="55">
         <v>1.1000000000000001</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="56">
+      <c r="C5" s="55">
         <v>0.75</v>
       </c>
-      <c r="D5" s="54">
+      <c r="D5" s="56">
         <v>0.75</v>
       </c>
-      <c r="E5" s="54"/>
+      <c r="E5" s="56"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="56"/>
+      <c r="A6" s="55"/>
       <c r="B6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="56"/>
+      <c r="A7" s="55"/>
       <c r="B7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="56"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="56"/>
+      <c r="A8" s="55"/>
       <c r="B8" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="56">
+      <c r="A9" s="55">
         <v>1.2</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="56">
+      <c r="C9" s="55">
         <v>1</v>
       </c>
-      <c r="D9" s="54">
+      <c r="D9" s="56">
         <v>1</v>
       </c>
-      <c r="E9" s="54"/>
+      <c r="E9" s="56"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="56"/>
+      <c r="A10" s="55"/>
       <c r="B10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="56"/>
+      <c r="A11" s="55"/>
       <c r="B11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="56"/>
+      <c r="A12" s="55"/>
       <c r="B12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="56"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="56"/>
+      <c r="A13" s="55"/>
       <c r="B13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="56"/>
+      <c r="A14" s="55"/>
       <c r="B14" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="56">
+      <c r="A15" s="55">
         <v>1.3</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="56">
+      <c r="C15" s="55">
         <v>1</v>
       </c>
-      <c r="D15" s="54">
+      <c r="D15" s="56">
         <v>0.75</v>
       </c>
-      <c r="E15" s="54"/>
+      <c r="E15" s="56"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="56"/>
+      <c r="A16" s="55"/>
       <c r="B16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="56"/>
+      <c r="A17" s="55"/>
       <c r="B17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="7">
@@ -1814,152 +1814,152 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="56">
+      <c r="A20" s="55">
         <v>2.1</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="56">
+      <c r="C20" s="55">
         <v>0.75</v>
       </c>
-      <c r="D20" s="54">
+      <c r="D20" s="56">
         <v>0.5</v>
       </c>
-      <c r="E20" s="54"/>
+      <c r="E20" s="56"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="56"/>
+      <c r="A21" s="55"/>
       <c r="B21" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="56"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="56"/>
+      <c r="A22" s="55"/>
       <c r="B22" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="56"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="58"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="56"/>
+      <c r="A23" s="55"/>
       <c r="B23" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="56">
+      <c r="A24" s="55">
         <v>2.2000000000000002</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="56">
+      <c r="C24" s="55">
         <v>0.5</v>
       </c>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="56"/>
+      <c r="A25" s="55"/>
       <c r="B25" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="56"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="56">
+      <c r="A26" s="55">
         <v>2.2999999999999998</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="56">
+      <c r="C26" s="55">
         <v>0.75</v>
       </c>
-      <c r="D26" s="54">
+      <c r="D26" s="56">
         <v>0.75</v>
       </c>
-      <c r="E26" s="54"/>
+      <c r="E26" s="56"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="56"/>
+      <c r="A27" s="55"/>
       <c r="B27" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="56"/>
+      <c r="A28" s="55"/>
       <c r="B28" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="56"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="56">
+      <c r="A29" s="55">
         <v>2.4</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="56">
+      <c r="C29" s="55">
         <v>1.5</v>
       </c>
-      <c r="D29" s="54">
+      <c r="D29" s="56">
         <v>1.5</v>
       </c>
-      <c r="E29" s="54"/>
+      <c r="E29" s="56"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="56"/>
+      <c r="A30" s="55"/>
       <c r="B30" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="56"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="56"/>
+      <c r="A31" s="55"/>
       <c r="B31" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="56"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="56"/>
+      <c r="A32" s="55"/>
       <c r="B32" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="56"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="55"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="7">
@@ -1981,13 +1981,13 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="57" t="s">
+      <c r="A34" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="57"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="57"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="58"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="7">
@@ -2033,110 +2033,110 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="57" t="s">
+      <c r="A38" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="57"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="57"/>
-      <c r="E38" s="57"/>
+      <c r="B38" s="58"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="58"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="56">
+      <c r="A39" s="55">
         <v>4.0999999999999996</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C39" s="56">
+      <c r="C39" s="55">
         <v>0.5</v>
       </c>
-      <c r="D39" s="54"/>
-      <c r="E39" s="54"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="56"/>
+      <c r="A40" s="55"/>
       <c r="B40" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="56"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="58"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="59"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="56"/>
+      <c r="A41" s="55"/>
       <c r="B41" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="56"/>
-      <c r="D41" s="55"/>
-      <c r="E41" s="55"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="56">
+      <c r="A42" s="55">
         <v>4.2</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C42" s="56">
+      <c r="C42" s="55">
         <v>1</v>
       </c>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="56"/>
+      <c r="A43" s="55"/>
       <c r="B43" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="56"/>
-      <c r="D43" s="55"/>
-      <c r="E43" s="55"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="56">
+      <c r="A44" s="55">
         <v>4.3</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="56">
+      <c r="C44" s="55">
         <v>0.5</v>
       </c>
-      <c r="D44" s="54"/>
-      <c r="E44" s="54"/>
+      <c r="D44" s="56"/>
+      <c r="E44" s="56"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="56"/>
+      <c r="A45" s="55"/>
       <c r="B45" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C45" s="56"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="56">
+      <c r="A46" s="55">
         <v>4.4000000000000004</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C46" s="56">
+      <c r="C46" s="55">
         <v>0.75</v>
       </c>
-      <c r="D46" s="54"/>
-      <c r="E46" s="54"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="56"/>
+      <c r="A47" s="55"/>
       <c r="B47" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C47" s="56"/>
-      <c r="D47" s="55"/>
-      <c r="E47" s="55"/>
+      <c r="C47" s="55"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
       <c r="F47">
         <f>SUM(D39:D47)</f>
         <v>0</v>
@@ -2162,6 +2162,39 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="A39:A41"/>
@@ -2178,39 +2211,6 @@
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="C29:C32"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="D5:D8"/>
-    <mergeCell ref="E5:E8"/>
-    <mergeCell ref="D9:D14"/>
-    <mergeCell ref="E9:E14"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C42:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Up lên các phân công tiếp theo:(lần 3) Các anh em cố lên nha. Coi bản phân công về nhà làm nha.
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -11,15 +11,15 @@
     <sheet name="DS Chức năng" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Phân công'!$B$1:$F$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Phân công'!$B$1:$F$31</definedName>
     <definedName name="OLE_LINK1" localSheetId="0">'Phân công'!$B$12</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="102">
   <si>
     <t>STT</t>
   </si>
@@ -283,9 +283,6 @@
   </si>
   <si>
     <t>Gửi email</t>
-  </si>
-  <si>
-    <t>Tiếp tục</t>
   </si>
   <si>
     <t>Mới</t>
@@ -314,39 +311,43 @@
     <t>x</t>
   </si>
   <si>
-    <t>Đaã thiết kế nhưng chưa biết làm sao</t>
-  </si>
-  <si>
     <t>Cần tạo địa chỉ gmail chung cho nhóm.</t>
   </si>
   <si>
     <t>Chưa làm được với web user control</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quản lý Banner/ logo/ theme: Thêm, Xóa, Sửa</t>
+  </si>
+  <si>
+    <t>Chưa xong</t>
+  </si>
+  <si>
+    <t>Đã thiết kế nhưng chưa biết làm sao</t>
+  </si>
+  <si>
+    <t>Chỉnh lại
+ danh mục 
+chính và 
+danh mục
+ phụ</t>
+  </si>
+  <si>
+    <t>Xem cái 
+demo email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -390,30 +391,56 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFFFF00"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="13"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="13"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -462,8 +489,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -551,145 +590,95 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -699,8 +688,90 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -712,11 +783,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1012,586 +1095,715 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12:H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.85546875" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41" style="57" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="47.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" ht="49.5">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75">
-      <c r="A2" s="12">
+    <row r="2" spans="1:8">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="30" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="16" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75">
-      <c r="A3" s="12">
+      <c r="G2" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="71" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="30" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:6" ht="30">
-      <c r="A4" s="12">
+      <c r="F3" s="16"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="70"/>
+    </row>
+    <row r="4" spans="1:8" ht="33">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="13">
         <v>1.2</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="16" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="30">
-      <c r="A5" s="12">
+      <c r="G4" s="58"/>
+      <c r="H4" s="70"/>
+    </row>
+    <row r="5" spans="1:8" ht="33">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="13">
         <v>1.2</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75">
-      <c r="A6" s="12">
+      <c r="G5" s="58"/>
+      <c r="H5" s="70"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="13">
         <v>1.2</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75">
-      <c r="A7" s="12">
+      <c r="F6" s="16"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="70"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="13">
         <v>1.2</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75">
-      <c r="A8" s="12">
+      <c r="G7" s="58"/>
+      <c r="H7" s="70"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="13">
         <v>1.2</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75">
-      <c r="A9" s="12">
+      <c r="F8" s="16"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="70"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="13">
         <v>1.3</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75">
-      <c r="A10" s="12">
+      <c r="F9" s="16"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="70"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="17">
         <v>9</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="17">
         <v>1.3</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="48" t="s">
+      <c r="E10" s="17"/>
+      <c r="F10" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="58"/>
+      <c r="H10" s="70"/>
+    </row>
+    <row r="11" spans="1:8" ht="33">
+      <c r="A11" s="21">
+        <v>10</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="19">
+        <v>4.2</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="58"/>
+      <c r="H11" s="70"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="13">
+        <v>12</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="72" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="13">
+        <v>13</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="59"/>
+      <c r="H13" s="69"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="13">
+        <v>14</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="25"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="69"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="13">
+        <v>15</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="25"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="69"/>
+    </row>
+    <row r="16" spans="1:8" ht="33">
+      <c r="A16" s="13">
+        <v>16</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" s="59"/>
+      <c r="H16" s="69"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="13">
+        <v>17</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="24">
+        <v>2.1</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" s="59"/>
+      <c r="H17" s="69"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="21">
+        <v>18</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="19">
+        <v>4.3</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="59"/>
+      <c r="H18" s="69"/>
+    </row>
+    <row r="19" spans="1:8" ht="33">
+      <c r="A19" s="13">
+        <v>20</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="28">
+        <v>2.4</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="60" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="33">
+      <c r="A20" s="13">
+        <v>21</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="32">
+        <v>2.4</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="60"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="15">
+        <v>22</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="32">
+        <v>1.4</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="60"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="15">
+        <v>23</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="32"/>
+      <c r="D22" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="60"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="34">
+        <v>24</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="34">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="34"/>
+      <c r="F23" s="36" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="31.5">
-      <c r="A11" s="30">
-        <v>10</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" s="42">
-        <v>4.2</v>
-      </c>
-      <c r="D11" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="43" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="12">
-        <v>12</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="18" t="s">
+      <c r="G23" s="60"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="13">
+        <v>25</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="38">
+        <v>2.4</v>
+      </c>
+      <c r="D24" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="12">
-        <v>13</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="18" t="s">
+      <c r="F24" s="39"/>
+      <c r="G24" s="61" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="13">
+        <v>26</v>
+      </c>
+      <c r="B25" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="38">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D25" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="40"/>
+      <c r="G25" s="61"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="13">
+        <v>27</v>
+      </c>
+      <c r="B26" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="38">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D26" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" s="40"/>
+      <c r="G26" s="61"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="21">
+        <v>28</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="19">
+        <v>3.2</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="19"/>
+      <c r="F27" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="G27" s="61"/>
+    </row>
+    <row r="28" spans="1:8" ht="33">
+      <c r="A28" s="34">
+        <v>28</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="34">
+        <v>3.1</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="34"/>
+      <c r="F28" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="61"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="13">
+        <v>30</v>
+      </c>
+      <c r="B29" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="42">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D29" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="12">
-        <v>14</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="18" t="s">
+      <c r="F29" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="62" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="13">
+        <v>31</v>
+      </c>
+      <c r="B30" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="42">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D30" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="20"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="12">
-        <v>15</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="18" t="s">
+      <c r="F30" s="44"/>
+      <c r="G30" s="62"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="13">
+        <v>32</v>
+      </c>
+      <c r="B31" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="46">
+        <v>2.5</v>
+      </c>
+      <c r="D31" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="20"/>
-    </row>
-    <row r="16" spans="1:6" ht="30">
-      <c r="A16" s="12">
-        <v>16</v>
-      </c>
-      <c r="B16" s="19" t="s">
+      <c r="F31" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" s="62"/>
+    </row>
+    <row r="32" spans="1:8" ht="49.5">
+      <c r="A32" s="21">
+        <v>33</v>
+      </c>
+      <c r="B32" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="50">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D32" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="51"/>
+      <c r="F32" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="G32" s="62"/>
+    </row>
+    <row r="33" spans="1:7" ht="43.5" customHeight="1">
+      <c r="A33" s="52">
         <v>34</v>
       </c>
-      <c r="C16" s="18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="F16" s="49" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="12">
-        <v>17</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="18">
-        <v>2.1</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="F17" s="49" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75">
-      <c r="A18" s="30">
-        <v>18</v>
-      </c>
-      <c r="B18" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="39">
-        <v>4.3</v>
-      </c>
-      <c r="D18" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="40"/>
-    </row>
-    <row r="19" spans="1:6" ht="30">
-      <c r="A19" s="12">
-        <v>20</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="21">
-        <v>2.4</v>
-      </c>
-      <c r="D19" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30">
-      <c r="A20" s="12">
-        <v>21</v>
-      </c>
-      <c r="B20" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="51">
-        <v>2.4</v>
-      </c>
-      <c r="D20" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75">
-      <c r="A21" s="30">
-        <v>22</v>
-      </c>
-      <c r="B21" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="51">
-        <v>1.4</v>
-      </c>
-      <c r="D21" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75">
-      <c r="A22" s="30">
-        <v>23</v>
-      </c>
-      <c r="B22" s="50" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="23" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="12">
-        <v>25</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="15">
-        <v>2.4</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="17"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="12">
-        <v>26</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="15">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="47" t="s">
+      <c r="B33" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="54">
+        <v>3.3</v>
+      </c>
+      <c r="D33" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="53"/>
+      <c r="F33" s="56" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="12">
-        <v>27</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="15">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="47" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75">
-      <c r="A26" s="30">
-        <v>28</v>
-      </c>
-      <c r="B26" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="36">
-        <v>3.2</v>
-      </c>
-      <c r="D26" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="37" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75">
-      <c r="A27" s="12">
-        <v>30</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="24">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D27" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75">
-      <c r="A28" s="12">
-        <v>31</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="24">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D28" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="26"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75">
-      <c r="A29" s="12">
-        <v>32</v>
-      </c>
-      <c r="B29" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="27">
-        <v>2.5</v>
-      </c>
-      <c r="D29" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="47.25">
-      <c r="A30" s="30">
-        <v>33</v>
-      </c>
-      <c r="B30" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="C30" s="32">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D30" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34" t="s">
-        <v>88</v>
-      </c>
+      <c r="G33" s="62"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:F29"/>
+  <autoFilter ref="B1:F31"/>
+  <mergeCells count="7">
+    <mergeCell ref="H2:H11"/>
+    <mergeCell ref="H12:H18"/>
+    <mergeCell ref="G2:G11"/>
+    <mergeCell ref="G12:G18"/>
+    <mergeCell ref="G19:G23"/>
+    <mergeCell ref="G24:G28"/>
+    <mergeCell ref="G29:G33"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1614,529 +1826,529 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="55">
+      <c r="A5" s="64">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="55">
+      <c r="C5" s="64">
         <v>0.75</v>
       </c>
-      <c r="D5" s="56">
+      <c r="D5" s="65">
         <v>0.75</v>
       </c>
-      <c r="E5" s="56"/>
+      <c r="E5" s="65"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="55"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="64"/>
+      <c r="B6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="55"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="64"/>
+      <c r="B7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="55"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="64"/>
+      <c r="B8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="55">
+      <c r="A9" s="64">
         <v>1.2</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="55">
+      <c r="C9" s="64">
         <v>1</v>
       </c>
-      <c r="D9" s="56">
+      <c r="D9" s="65">
         <v>1</v>
       </c>
-      <c r="E9" s="56"/>
+      <c r="E9" s="65"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="55"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="64"/>
+      <c r="B10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="55"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="55"/>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="64"/>
+      <c r="B11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="55"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="55"/>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="64"/>
+      <c r="B12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="55"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="55"/>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="64"/>
+      <c r="B13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="55"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="55"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="64"/>
+      <c r="B14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="55"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="55">
+      <c r="A15" s="64">
         <v>1.3</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="55">
+      <c r="C15" s="64">
         <v>1</v>
       </c>
-      <c r="D15" s="56">
+      <c r="D15" s="65">
         <v>0.75</v>
       </c>
-      <c r="E15" s="56"/>
+      <c r="E15" s="65"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="55"/>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="64"/>
+      <c r="B16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="55"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="55"/>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="64"/>
+      <c r="B17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="55"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="7">
+      <c r="A18" s="5">
         <v>1.4</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="5">
         <v>0.5</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="5">
         <v>0.5</v>
       </c>
-      <c r="E18" s="7"/>
+      <c r="E18" s="5"/>
       <c r="F18">
         <f>SUM(D5:D18)</f>
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="55">
+      <c r="A20" s="64">
         <v>2.1</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="55">
+      <c r="C20" s="64">
         <v>0.75</v>
       </c>
-      <c r="D20" s="56">
+      <c r="D20" s="65">
         <v>0.5</v>
       </c>
-      <c r="E20" s="56"/>
+      <c r="E20" s="65"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="55"/>
-      <c r="B21" s="4" t="s">
+      <c r="A21" s="64"/>
+      <c r="B21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="55"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="55"/>
-      <c r="B22" s="4" t="s">
+      <c r="A22" s="64"/>
+      <c r="B22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="55"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="59"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="55"/>
-      <c r="B23" s="6" t="s">
+      <c r="A23" s="64"/>
+      <c r="B23" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="55"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="55">
+      <c r="A24" s="64">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="55">
+      <c r="C24" s="64">
         <v>0.5</v>
       </c>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="55"/>
-      <c r="B25" s="4" t="s">
+      <c r="A25" s="64"/>
+      <c r="B25" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="55"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="55">
+      <c r="A26" s="64">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="55">
+      <c r="C26" s="64">
         <v>0.75</v>
       </c>
-      <c r="D26" s="56">
+      <c r="D26" s="65">
         <v>0.75</v>
       </c>
-      <c r="E26" s="56"/>
+      <c r="E26" s="65"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="55"/>
-      <c r="B27" s="4" t="s">
+      <c r="A27" s="64"/>
+      <c r="B27" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="55"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="55"/>
-      <c r="B28" s="4" t="s">
+      <c r="A28" s="64"/>
+      <c r="B28" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="55"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="55">
+      <c r="A29" s="64">
         <v>2.4</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="55">
+      <c r="C29" s="64">
         <v>1.5</v>
       </c>
-      <c r="D29" s="56">
+      <c r="D29" s="65">
         <v>1.5</v>
       </c>
-      <c r="E29" s="56"/>
+      <c r="E29" s="65"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="55"/>
-      <c r="B30" s="4" t="s">
+      <c r="A30" s="64"/>
+      <c r="B30" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="55"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="68"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="55"/>
-      <c r="B31" s="4" t="s">
+      <c r="A31" s="64"/>
+      <c r="B31" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="55"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="55"/>
-      <c r="B32" s="4" t="s">
+      <c r="A32" s="64"/>
+      <c r="B32" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="55"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="57"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="66"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="7">
+      <c r="A33" s="5">
         <v>2.5</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="5">
         <v>0.5</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="5">
         <v>0.5</v>
       </c>
-      <c r="E33" s="7"/>
+      <c r="E33" s="5"/>
       <c r="F33">
         <f>SUM(D20:D33)</f>
         <v>3.25</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="58" t="s">
+      <c r="A34" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="58"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="67"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="67"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="7">
+      <c r="A35" s="5">
         <v>3.1</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="5">
         <v>0.5</v>
       </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="7">
+      <c r="A36" s="5">
         <v>3.2</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="5">
         <v>0.5</v>
       </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="7">
+      <c r="A37" s="5">
         <v>3.3</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="5">
         <v>0.5</v>
       </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
       <c r="F37">
         <f>SUM(D35:D37)</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="58" t="s">
+      <c r="A38" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="58"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
+      <c r="B38" s="67"/>
+      <c r="C38" s="67"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="67"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="55">
+      <c r="A39" s="64">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C39" s="55">
+      <c r="C39" s="64">
         <v>0.5</v>
       </c>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="65"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="55"/>
-      <c r="B40" s="4" t="s">
+      <c r="A40" s="64"/>
+      <c r="B40" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="55"/>
-      <c r="D40" s="59"/>
-      <c r="E40" s="59"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="68"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="55"/>
-      <c r="B41" s="4" t="s">
+      <c r="A41" s="64"/>
+      <c r="B41" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="55"/>
-      <c r="D41" s="57"/>
-      <c r="E41" s="57"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="66"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="55">
+      <c r="A42" s="64">
         <v>4.2</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C42" s="55">
+      <c r="C42" s="64">
         <v>1</v>
       </c>
-      <c r="D42" s="56"/>
-      <c r="E42" s="56"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="65"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="55"/>
-      <c r="B43" s="4" t="s">
+      <c r="A43" s="64"/>
+      <c r="B43" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="55"/>
-      <c r="D43" s="57"/>
-      <c r="E43" s="57"/>
+      <c r="C43" s="64"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="55">
+      <c r="A44" s="64">
         <v>4.3</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="55">
+      <c r="C44" s="64">
         <v>0.5</v>
       </c>
-      <c r="D44" s="56"/>
-      <c r="E44" s="56"/>
+      <c r="D44" s="65"/>
+      <c r="E44" s="65"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="55"/>
-      <c r="B45" s="4" t="s">
+      <c r="A45" s="64"/>
+      <c r="B45" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C45" s="55"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="57"/>
+      <c r="C45" s="64"/>
+      <c r="D45" s="66"/>
+      <c r="E45" s="66"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="55">
+      <c r="A46" s="64">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C46" s="55">
+      <c r="C46" s="64">
         <v>0.75</v>
       </c>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
+      <c r="D46" s="65"/>
+      <c r="E46" s="65"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="55"/>
-      <c r="B47" s="4" t="s">
+      <c r="A47" s="64"/>
+      <c r="B47" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C47" s="55"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
+      <c r="C47" s="64"/>
+      <c r="D47" s="66"/>
+      <c r="E47" s="66"/>
       <c r="F47">
         <f>SUM(D39:D47)</f>
         <v>0</v>
@@ -2152,7 +2364,7 @@
       </c>
     </row>
     <row r="49" spans="6:7">
-      <c r="F49" s="53">
+      <c r="F49" s="10">
         <f>F48*G49/G48</f>
         <v>2.34375</v>
       </c>

</xml_diff>

<commit_message>
Chỉnh sửa CSDL/WEBRAOVAT.sql - Thêm các câu lệnh insert logo, banner, giao diện ở cuối file. Xử lý giao diện từ CSDL. Xử lý xong chức năng phần banner và logo. Thêm image ở trên thanh URL. Bỏ cột chỉnh sửa ở trang chủ. Cập nhật Features.xlsx.
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Phân công" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Phân công'!$B$1:$F$31</definedName>
     <definedName name="OLE_LINK1" localSheetId="0">'Phân công'!$B$12</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="103">
   <si>
     <t>STT</t>
   </si>
@@ -336,12 +336,15 @@
     <t>Xem cái 
 demo email</t>
   </si>
+  <si>
+    <t>Chưa chọn Theme</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,6 +441,13 @@
       <color rgb="FFFFFF00"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -600,10 +610,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -756,6 +767,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -771,39 +794,40 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1097,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12:H18"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1149,10 +1173,10 @@
       <c r="F2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="71" t="s">
+      <c r="H2" s="58" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1171,8 +1195,8 @@
         <v>20</v>
       </c>
       <c r="F3" s="16"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="70"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="59"/>
     </row>
     <row r="4" spans="1:8" ht="33">
       <c r="A4" s="13">
@@ -1193,8 +1217,8 @@
       <c r="F4" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="58"/>
-      <c r="H4" s="70"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="59"/>
     </row>
     <row r="5" spans="1:8" ht="33">
       <c r="A5" s="13">
@@ -1215,8 +1239,8 @@
       <c r="F5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="58"/>
-      <c r="H5" s="70"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="59"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="13">
@@ -1235,8 +1259,8 @@
         <v>20</v>
       </c>
       <c r="F6" s="16"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="70"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="59"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="13">
@@ -1257,8 +1281,8 @@
       <c r="F7" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="58"/>
-      <c r="H7" s="70"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="59"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="13">
@@ -1277,8 +1301,8 @@
         <v>20</v>
       </c>
       <c r="F8" s="16"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="70"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="59"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="13">
@@ -1297,8 +1321,8 @@
         <v>20</v>
       </c>
       <c r="F9" s="16"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="70"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="59"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="17">
@@ -1317,8 +1341,8 @@
       <c r="F10" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="G10" s="58"/>
-      <c r="H10" s="70"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="59"/>
     </row>
     <row r="11" spans="1:8" ht="33">
       <c r="A11" s="21">
@@ -1337,8 +1361,8 @@
       <c r="F11" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="G11" s="58"/>
-      <c r="H11" s="70"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="59"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="13">
@@ -1359,10 +1383,10 @@
       <c r="F12" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="59" t="s">
+      <c r="G12" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="72" t="s">
+      <c r="H12" s="60" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1385,8 +1409,8 @@
       <c r="F13" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="G13" s="59"/>
-      <c r="H13" s="69"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="61"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="13">
@@ -1405,8 +1429,8 @@
         <v>20</v>
       </c>
       <c r="F14" s="25"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="69"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="61"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="13">
@@ -1425,8 +1449,8 @@
         <v>20</v>
       </c>
       <c r="F15" s="25"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="69"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="61"/>
     </row>
     <row r="16" spans="1:8" ht="33">
       <c r="A16" s="13">
@@ -1447,8 +1471,8 @@
       <c r="F16" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="59"/>
-      <c r="H16" s="69"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="61"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="13">
@@ -1469,8 +1493,8 @@
       <c r="F17" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="G17" s="59"/>
-      <c r="H17" s="69"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="61"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="21">
@@ -1489,8 +1513,8 @@
       <c r="F18" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="G18" s="59"/>
-      <c r="H18" s="69"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="61"/>
     </row>
     <row r="19" spans="1:8" ht="33">
       <c r="A19" s="13">
@@ -1511,7 +1535,7 @@
       <c r="F19" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="60" t="s">
+      <c r="G19" s="64" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1534,7 +1558,7 @@
       <c r="F20" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="60"/>
+      <c r="G20" s="64"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="15">
@@ -1555,7 +1579,7 @@
       <c r="F21" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="G21" s="60"/>
+      <c r="G21" s="64"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="15">
@@ -1574,7 +1598,7 @@
       <c r="F22" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="G22" s="60"/>
+      <c r="G22" s="64"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="34">
@@ -1591,9 +1615,9 @@
       </c>
       <c r="E23" s="34"/>
       <c r="F23" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="G23" s="60"/>
+        <v>102</v>
+      </c>
+      <c r="G23" s="64"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="13">
@@ -1612,7 +1636,7 @@
         <v>20</v>
       </c>
       <c r="F24" s="39"/>
-      <c r="G24" s="61" t="s">
+      <c r="G24" s="65" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1633,7 +1657,7 @@
         <v>94</v>
       </c>
       <c r="F25" s="40"/>
-      <c r="G25" s="61"/>
+      <c r="G25" s="65"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="13">
@@ -1652,7 +1676,7 @@
         <v>94</v>
       </c>
       <c r="F26" s="40"/>
-      <c r="G26" s="61"/>
+      <c r="G26" s="65"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="21">
@@ -1671,7 +1695,7 @@
       <c r="F27" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="G27" s="61"/>
+      <c r="G27" s="65"/>
     </row>
     <row r="28" spans="1:8" ht="33">
       <c r="A28" s="34">
@@ -1690,7 +1714,7 @@
       <c r="F28" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="G28" s="61"/>
+      <c r="G28" s="65"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="13">
@@ -1711,7 +1735,7 @@
       <c r="F29" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="G29" s="62" t="s">
+      <c r="G29" s="66" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1732,7 +1756,7 @@
         <v>20</v>
       </c>
       <c r="F30" s="44"/>
-      <c r="G30" s="62"/>
+      <c r="G30" s="66"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="13">
@@ -1753,7 +1777,7 @@
       <c r="F31" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="G31" s="62"/>
+      <c r="G31" s="66"/>
     </row>
     <row r="32" spans="1:8" ht="49.5">
       <c r="A32" s="21">
@@ -1772,7 +1796,7 @@
       <c r="F32" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="G32" s="62"/>
+      <c r="G32" s="66"/>
     </row>
     <row r="33" spans="1:7" ht="43.5" customHeight="1">
       <c r="A33" s="52">
@@ -1791,18 +1815,18 @@
       <c r="F33" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="G33" s="62"/>
+      <c r="G33" s="66"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:F31"/>
   <mergeCells count="7">
+    <mergeCell ref="G24:G28"/>
+    <mergeCell ref="G29:G33"/>
     <mergeCell ref="H2:H11"/>
     <mergeCell ref="H12:H18"/>
     <mergeCell ref="G2:G11"/>
     <mergeCell ref="G12:G18"/>
     <mergeCell ref="G19:G23"/>
-    <mergeCell ref="G24:G28"/>
-    <mergeCell ref="G29:G33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1813,8 +1837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46:D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1826,13 +1850,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
@@ -1863,148 +1887,148 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="64">
+      <c r="A5" s="69">
         <v>1.1000000000000001</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="64">
+      <c r="C5" s="69">
         <v>0.75</v>
       </c>
-      <c r="D5" s="65">
+      <c r="D5" s="73">
         <v>0.75</v>
       </c>
-      <c r="E5" s="65"/>
+      <c r="E5" s="67"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="64"/>
+      <c r="A6" s="69"/>
       <c r="B6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="64"/>
+      <c r="A7" s="69"/>
       <c r="B7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="64"/>
+      <c r="A8" s="69"/>
       <c r="B8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="64">
+      <c r="A9" s="69">
         <v>1.2</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="64">
+      <c r="C9" s="69">
         <v>1</v>
       </c>
-      <c r="D9" s="65">
+      <c r="D9" s="73">
         <v>1</v>
       </c>
-      <c r="E9" s="65"/>
+      <c r="E9" s="67"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="64"/>
+      <c r="A10" s="69"/>
       <c r="B10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="64"/>
+      <c r="A11" s="69"/>
       <c r="B11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="68"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="64"/>
+      <c r="A12" s="69"/>
       <c r="B12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="68"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="64"/>
+      <c r="A13" s="69"/>
       <c r="B13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="64"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="64"/>
+      <c r="A14" s="69"/>
       <c r="B14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="64"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="64">
+      <c r="A15" s="69">
         <v>1.3</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="64">
+      <c r="C15" s="69">
         <v>1</v>
       </c>
-      <c r="D15" s="65">
+      <c r="D15" s="73">
         <v>0.75</v>
       </c>
-      <c r="E15" s="65"/>
+      <c r="E15" s="67"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="64"/>
+      <c r="A16" s="69"/>
       <c r="B16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="64"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="71"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="64"/>
+      <c r="A17" s="69"/>
       <c r="B17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="64"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="5">
@@ -2016,162 +2040,164 @@
       <c r="C18" s="5">
         <v>0.5</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="74">
         <v>0.5</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18">
-        <f>SUM(D5:D18)</f>
-        <v>3</v>
+        <f>C5*D5+C9*D9+C15*D15+C18*D18</f>
+        <v>2.5625</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="67" t="s">
+      <c r="A19" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="64">
+      <c r="A20" s="69">
         <v>2.1</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="64">
+      <c r="C20" s="69">
         <v>0.75</v>
       </c>
-      <c r="D20" s="65">
-        <v>0.5</v>
-      </c>
-      <c r="E20" s="65"/>
+      <c r="D20" s="73">
+        <v>1</v>
+      </c>
+      <c r="E20" s="67"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="64"/>
+      <c r="A21" s="69"/>
       <c r="B21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="64"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="68"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="64"/>
+      <c r="A22" s="69"/>
       <c r="B22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="64"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="64"/>
+      <c r="A23" s="69"/>
       <c r="B23" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="64">
+      <c r="A24" s="69">
         <v>2.2000000000000002</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="64">
+      <c r="C24" s="69">
         <v>0.5</v>
       </c>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
+      <c r="D24" s="73">
+        <v>1</v>
+      </c>
+      <c r="E24" s="67"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="64"/>
+      <c r="A25" s="69"/>
       <c r="B25" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="64"/>
-      <c r="D25" s="66"/>
-      <c r="E25" s="66"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="64">
+      <c r="A26" s="69">
         <v>2.2999999999999998</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="64">
+      <c r="C26" s="69">
         <v>0.75</v>
       </c>
-      <c r="D26" s="65">
-        <v>0.75</v>
-      </c>
-      <c r="E26" s="65"/>
+      <c r="D26" s="73">
+        <v>1</v>
+      </c>
+      <c r="E26" s="67"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="64"/>
+      <c r="A27" s="69"/>
       <c r="B27" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="64"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="64"/>
+      <c r="A28" s="69"/>
       <c r="B28" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="64"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="64">
+      <c r="A29" s="69">
         <v>2.4</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="64">
+      <c r="C29" s="69">
         <v>1.5</v>
       </c>
-      <c r="D29" s="65">
-        <v>1.5</v>
-      </c>
-      <c r="E29" s="65"/>
+      <c r="D29" s="73">
+        <v>1</v>
+      </c>
+      <c r="E29" s="67"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="64"/>
+      <c r="A30" s="69"/>
       <c r="B30" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="64"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="68"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="64"/>
+      <c r="A31" s="69"/>
       <c r="B31" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="64"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="68"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="64"/>
+      <c r="A32" s="69"/>
       <c r="B32" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="64"/>
-      <c r="D32" s="66"/>
-      <c r="E32" s="66"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="68"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="5">
@@ -2183,23 +2209,23 @@
       <c r="C33" s="5">
         <v>0.5</v>
       </c>
-      <c r="D33" s="5">
-        <v>0.5</v>
+      <c r="D33" s="74">
+        <v>1</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33">
-        <f>SUM(D20:D33)</f>
-        <v>3.25</v>
+        <f>C20*D20+C24*D24+C26*D26+C29*D29+C33*D33</f>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="67" t="s">
+      <c r="A34" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="67"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="67"/>
+      <c r="B34" s="70"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="5">
@@ -2211,7 +2237,9 @@
       <c r="C35" s="5">
         <v>0.5</v>
       </c>
-      <c r="D35" s="5"/>
+      <c r="D35" s="74">
+        <v>0</v>
+      </c>
       <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:7">
@@ -2224,7 +2252,9 @@
       <c r="C36" s="5">
         <v>0.5</v>
       </c>
-      <c r="D36" s="5"/>
+      <c r="D36" s="74">
+        <v>0</v>
+      </c>
       <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:7">
@@ -2237,127 +2267,137 @@
       <c r="C37" s="5">
         <v>0.5</v>
       </c>
-      <c r="D37" s="5"/>
+      <c r="D37" s="74">
+        <v>0</v>
+      </c>
       <c r="E37" s="5"/>
       <c r="F37">
-        <f>SUM(D35:D37)</f>
+        <f>C35*D35+C36*D36+C37*D37</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="67" t="s">
+      <c r="A38" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="67"/>
-      <c r="C38" s="67"/>
-      <c r="D38" s="67"/>
-      <c r="E38" s="67"/>
+      <c r="B38" s="70"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="70"/>
+      <c r="E38" s="70"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="64">
+      <c r="A39" s="69">
         <v>4.0999999999999996</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C39" s="64">
+      <c r="C39" s="69">
         <v>0.5</v>
       </c>
-      <c r="D39" s="65"/>
-      <c r="E39" s="65"/>
+      <c r="D39" s="73">
+        <v>0.25</v>
+      </c>
+      <c r="E39" s="67"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="64"/>
+      <c r="A40" s="69"/>
       <c r="B40" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="64"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="68"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="71"/>
+      <c r="E40" s="71"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="64"/>
+      <c r="A41" s="69"/>
       <c r="B41" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="64"/>
-      <c r="D41" s="66"/>
-      <c r="E41" s="66"/>
+      <c r="C41" s="69"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="64">
+      <c r="A42" s="69">
         <v>4.2</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C42" s="64">
+      <c r="C42" s="69">
         <v>1</v>
       </c>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
+      <c r="D42" s="75">
+        <v>0</v>
+      </c>
+      <c r="E42" s="67"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="64"/>
+      <c r="A43" s="69"/>
       <c r="B43" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="64"/>
-      <c r="D43" s="66"/>
-      <c r="E43" s="66"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="76"/>
+      <c r="E43" s="68"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="64">
+      <c r="A44" s="69">
         <v>4.3</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="64">
+      <c r="C44" s="69">
         <v>0.5</v>
       </c>
-      <c r="D44" s="65"/>
-      <c r="E44" s="65"/>
+      <c r="D44" s="75">
+        <v>0</v>
+      </c>
+      <c r="E44" s="67"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="64"/>
+      <c r="A45" s="69"/>
       <c r="B45" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C45" s="64"/>
-      <c r="D45" s="66"/>
-      <c r="E45" s="66"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="76"/>
+      <c r="E45" s="68"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="64">
+      <c r="A46" s="69">
         <v>4.4000000000000004</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C46" s="64">
+      <c r="C46" s="69">
         <v>0.75</v>
       </c>
-      <c r="D46" s="65"/>
-      <c r="E46" s="65"/>
+      <c r="D46" s="73">
+        <v>0.75</v>
+      </c>
+      <c r="E46" s="67"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="64"/>
+      <c r="A47" s="69"/>
       <c r="B47" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C47" s="64"/>
-      <c r="D47" s="66"/>
-      <c r="E47" s="66"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="68"/>
+      <c r="E47" s="68"/>
       <c r="F47">
-        <f>SUM(D39:D47)</f>
-        <v>0</v>
+        <f>C39*D39+C42*D42+C44*D44+C46*D46</f>
+        <v>0.6875</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="F48">
         <f>SUM(F5:F47)</f>
-        <v>6.25</v>
+        <v>7.25</v>
       </c>
       <c r="G48">
         <v>10</v>
@@ -2366,7 +2406,7 @@
     <row r="49" spans="6:7">
       <c r="F49" s="10">
         <f>F48*G49/G48</f>
-        <v>2.34375</v>
+        <v>2.71875</v>
       </c>
       <c r="G49">
         <v>3.75</v>
@@ -2374,23 +2414,22 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="D5:D8"/>
-    <mergeCell ref="E5:E8"/>
-    <mergeCell ref="D9:D14"/>
-    <mergeCell ref="E9:E14"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="C29:C32"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A46:A47"/>
@@ -2407,22 +2446,23 @@
     <mergeCell ref="E42:E43"/>
     <mergeCell ref="D20:D23"/>
     <mergeCell ref="E20:E23"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C42:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Chỉnh sửa giao diện Default và Master Page. Chuyển ngữ Default và Master Page. Chỉnh sửa TRV mới nhất (trang chủ).
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="102">
   <si>
     <t>STT</t>
   </si>
@@ -320,19 +320,16 @@
     <t>Giao diện chưa đẹp</t>
   </si>
   <si>
-    <t>Bị lỗi cột bên trái</t>
-  </si>
-  <si>
     <t>Hoàn chỉnh tuy chưa đẹp</t>
   </si>
   <si>
-    <t>Tích hợp hoàn chỉnh</t>
-  </si>
-  <si>
     <t>Không có FileUpload filter.</t>
   </si>
   <si>
     <t>Quản lý Banner/ logo/ theme: Thêm, Xóa, Sửa</t>
+  </si>
+  <si>
+    <t>Tích hợp hoàn chỉnh, chưa bỏ trang Tìm Kiếm bên ngoài</t>
   </si>
 </sst>
 </file>
@@ -754,6 +751,30 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -781,55 +802,31 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1144,28 +1141,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="81" t="s">
+      <c r="F1" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="81" t="s">
+      <c r="G1" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="76"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="21">
@@ -1181,16 +1178,16 @@
       <c r="E2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="74">
+      <c r="F2" s="56">
         <v>1</v>
       </c>
       <c r="G2" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="H2" s="62" t="s">
+      <c r="H2" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="58"/>
+      <c r="I2" s="66"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="21">
@@ -1210,8 +1207,8 @@
       <c r="G3" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="H3" s="62"/>
-      <c r="I3" s="59"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="21">
@@ -1229,14 +1226,14 @@
       <c r="E4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="74">
+      <c r="F4" s="56">
         <v>1</v>
       </c>
       <c r="G4" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="H4" s="62"/>
-      <c r="I4" s="59"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="67"/>
     </row>
     <row r="5" spans="1:9" ht="33">
       <c r="A5" s="21">
@@ -1254,12 +1251,14 @@
       <c r="E5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="56">
+        <v>1</v>
+      </c>
       <c r="G5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="62"/>
-      <c r="I5" s="59"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="67"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="21">
@@ -1277,14 +1276,14 @@
       <c r="E6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="74">
+      <c r="F6" s="56">
         <v>1</v>
       </c>
       <c r="G6" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="H6" s="62"/>
-      <c r="I6" s="59"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="67"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="21">
@@ -1302,12 +1301,14 @@
       <c r="E7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="56">
+        <v>1</v>
+      </c>
       <c r="G7" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="H7" s="62"/>
-      <c r="I7" s="59"/>
+        <v>96</v>
+      </c>
+      <c r="H7" s="70"/>
+      <c r="I7" s="67"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="21">
@@ -1325,16 +1326,16 @@
       <c r="E8" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="74">
+      <c r="F8" s="56">
         <v>1</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="H8" s="62"/>
-      <c r="I8" s="59"/>
-    </row>
-    <row r="9" spans="1:9">
+        <v>98</v>
+      </c>
+      <c r="H8" s="70"/>
+      <c r="I8" s="67"/>
+    </row>
+    <row r="9" spans="1:9" ht="33">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -1350,14 +1351,14 @@
       <c r="E9" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="74">
+      <c r="F9" s="56">
         <v>1</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="H9" s="62"/>
-      <c r="I9" s="59"/>
+        <v>101</v>
+      </c>
+      <c r="H9" s="70"/>
+      <c r="I9" s="67"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="25">
@@ -1377,8 +1378,8 @@
       <c r="G10" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="H10" s="62"/>
-      <c r="I10" s="59"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="67"/>
     </row>
     <row r="11" spans="1:9" ht="33">
       <c r="A11" s="23">
@@ -1398,8 +1399,8 @@
       <c r="G11" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="H11" s="62"/>
-      <c r="I11" s="59"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="67"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="14">
@@ -1421,10 +1422,10 @@
       <c r="G12" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="H12" s="63" t="s">
+      <c r="H12" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="60"/>
+      <c r="I12" s="68"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="14">
@@ -1446,8 +1447,8 @@
       <c r="G13" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="H13" s="63"/>
-      <c r="I13" s="61"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="69"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="14">
@@ -1467,8 +1468,8 @@
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="16"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="61"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="69"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="14">
@@ -1488,8 +1489,8 @@
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="16"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="61"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="69"/>
     </row>
     <row r="16" spans="1:9" ht="33">
       <c r="A16" s="14">
@@ -1511,8 +1512,8 @@
       <c r="G16" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="H16" s="63"/>
-      <c r="I16" s="61"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="69"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="14">
@@ -1534,8 +1535,8 @@
       <c r="G17" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="H17" s="63"/>
-      <c r="I17" s="61"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="69"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="18">
@@ -1555,8 +1556,8 @@
       <c r="G18" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="H18" s="63"/>
-      <c r="I18" s="61"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="69"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="30">
@@ -1576,9 +1577,9 @@
       </c>
       <c r="F19" s="30"/>
       <c r="G19" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="H19" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19" s="72" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1600,9 +1601,9 @@
       </c>
       <c r="F20" s="35"/>
       <c r="G20" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="H20" s="64"/>
+        <v>99</v>
+      </c>
+      <c r="H20" s="72"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="32">
@@ -1622,7 +1623,7 @@
       </c>
       <c r="F21" s="36"/>
       <c r="G21" s="33"/>
-      <c r="H21" s="64"/>
+      <c r="H21" s="72"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="32">
@@ -1640,14 +1641,14 @@
       </c>
       <c r="F22" s="36"/>
       <c r="G22" s="33"/>
-      <c r="H22" s="64"/>
+      <c r="H22" s="72"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="35">
         <v>24</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C23" s="35">
         <v>4.4000000000000004</v>
@@ -1659,10 +1660,10 @@
         <v>20</v>
       </c>
       <c r="F23" s="35"/>
-      <c r="G23" s="75" t="s">
+      <c r="G23" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="H23" s="64"/>
+      <c r="H23" s="72"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="37">
@@ -1682,7 +1683,7 @@
       </c>
       <c r="F24" s="37"/>
       <c r="G24" s="39"/>
-      <c r="H24" s="56" t="s">
+      <c r="H24" s="64" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1704,7 +1705,7 @@
       </c>
       <c r="F25" s="37"/>
       <c r="G25" s="40"/>
-      <c r="H25" s="56"/>
+      <c r="H25" s="64"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="37">
@@ -1724,7 +1725,7 @@
       </c>
       <c r="F26" s="37"/>
       <c r="G26" s="40"/>
-      <c r="H26" s="56"/>
+      <c r="H26" s="64"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="41">
@@ -1744,7 +1745,7 @@
       <c r="G27" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="H27" s="56"/>
+      <c r="H27" s="64"/>
     </row>
     <row r="28" spans="1:9" ht="33">
       <c r="A28" s="46">
@@ -1764,7 +1765,7 @@
       <c r="G28" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="H28" s="56"/>
+      <c r="H28" s="64"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="49">
@@ -1786,7 +1787,7 @@
       <c r="G29" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="H29" s="57" t="s">
+      <c r="H29" s="65" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1808,7 +1809,7 @@
       </c>
       <c r="F30" s="49"/>
       <c r="G30" s="52"/>
-      <c r="H30" s="57"/>
+      <c r="H30" s="65"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="49">
@@ -1830,13 +1831,13 @@
       <c r="G31" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="H31" s="57"/>
+      <c r="H31" s="65"/>
     </row>
     <row r="32" spans="1:9" ht="49.5">
       <c r="A32" s="45">
         <v>33</v>
       </c>
-      <c r="B32" s="77" t="s">
+      <c r="B32" s="59" t="s">
         <v>86</v>
       </c>
       <c r="C32" s="45">
@@ -1845,18 +1846,18 @@
       <c r="D32" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="E32" s="78"/>
-      <c r="F32" s="78"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="H32" s="57"/>
+      <c r="H32" s="65"/>
     </row>
     <row r="33" spans="1:8" ht="43.5" customHeight="1">
       <c r="A33" s="54">
         <v>34</v>
       </c>
-      <c r="B33" s="79" t="s">
+      <c r="B33" s="61" t="s">
         <v>72</v>
       </c>
       <c r="C33" s="54">
@@ -1865,12 +1866,12 @@
       <c r="D33" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="79"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="80" t="s">
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="H33" s="57"/>
+      <c r="H33" s="65"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:G31">
@@ -1944,148 +1945,148 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="70">
+      <c r="A5" s="74">
         <v>1.1000000000000001</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="70">
+      <c r="C5" s="74">
         <v>0.75</v>
       </c>
-      <c r="D5" s="69">
+      <c r="D5" s="75">
         <v>0.75</v>
       </c>
-      <c r="E5" s="67"/>
+      <c r="E5" s="79"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="70"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="70"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="70"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="70"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="70"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="70">
+      <c r="A9" s="74">
         <v>1.2</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="70">
+      <c r="C9" s="74">
         <v>1</v>
       </c>
-      <c r="D9" s="69">
+      <c r="D9" s="75">
         <v>1</v>
       </c>
-      <c r="E9" s="67"/>
+      <c r="E9" s="79"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="70"/>
+      <c r="A10" s="74"/>
       <c r="B10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="70"/>
+      <c r="A11" s="74"/>
       <c r="B11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="70"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="70"/>
+      <c r="A12" s="74"/>
       <c r="B12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="70"/>
+      <c r="A13" s="74"/>
       <c r="B13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="70"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="70"/>
+      <c r="A14" s="74"/>
       <c r="B14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="70"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="70">
+      <c r="A15" s="74">
         <v>1.3</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="70">
+      <c r="C15" s="74">
         <v>1</v>
       </c>
-      <c r="D15" s="69">
+      <c r="D15" s="75">
         <v>0.75</v>
       </c>
-      <c r="E15" s="67"/>
+      <c r="E15" s="79"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="70"/>
+      <c r="A16" s="74"/>
       <c r="B16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="70"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="70"/>
+      <c r="A17" s="74"/>
       <c r="B17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="70"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="68"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="5">
@@ -2107,154 +2108,154 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="71" t="s">
+      <c r="A19" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="71"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
+      <c r="B19" s="77"/>
+      <c r="C19" s="77"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="70">
+      <c r="A20" s="74">
         <v>2.1</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="70">
+      <c r="C20" s="74">
         <v>0.75</v>
       </c>
-      <c r="D20" s="69">
+      <c r="D20" s="75">
         <v>1</v>
       </c>
-      <c r="E20" s="67"/>
+      <c r="E20" s="79"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="70"/>
+      <c r="A21" s="74"/>
       <c r="B21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="70"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="78"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="70"/>
+      <c r="A22" s="74"/>
       <c r="B22" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="70"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="78"/>
+      <c r="E22" s="78"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="70"/>
+      <c r="A23" s="74"/>
       <c r="B23" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="70"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="68"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="70">
+      <c r="A24" s="74">
         <v>2.2000000000000002</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="70">
+      <c r="C24" s="74">
         <v>0.5</v>
       </c>
-      <c r="D24" s="69">
+      <c r="D24" s="75">
         <v>1</v>
       </c>
-      <c r="E24" s="67"/>
+      <c r="E24" s="79"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="70"/>
+      <c r="A25" s="74"/>
       <c r="B25" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="70"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="68"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="76"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="70">
+      <c r="A26" s="74">
         <v>2.2999999999999998</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="70">
+      <c r="C26" s="74">
         <v>0.75</v>
       </c>
-      <c r="D26" s="69">
+      <c r="D26" s="75">
         <v>1</v>
       </c>
-      <c r="E26" s="67"/>
+      <c r="E26" s="79"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="70"/>
+      <c r="A27" s="74"/>
       <c r="B27" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="70"/>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
+      <c r="C27" s="74"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="78"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="70"/>
+      <c r="A28" s="74"/>
       <c r="B28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="70"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="68"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="76"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="70">
+      <c r="A29" s="74">
         <v>2.4</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="70">
+      <c r="C29" s="74">
         <v>1.5</v>
       </c>
-      <c r="D29" s="69">
+      <c r="D29" s="75">
         <v>1</v>
       </c>
-      <c r="E29" s="67"/>
+      <c r="E29" s="79"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="70"/>
+      <c r="A30" s="74"/>
       <c r="B30" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="70"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="72"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="78"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="70"/>
+      <c r="A31" s="74"/>
       <c r="B31" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="70"/>
-      <c r="D31" s="72"/>
-      <c r="E31" s="72"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="78"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="70"/>
+      <c r="A32" s="74"/>
       <c r="B32" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="70"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="68"/>
+      <c r="C32" s="74"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="76"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="5">
@@ -2276,13 +2277,13 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="71" t="s">
+      <c r="A34" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="71"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="71"/>
+      <c r="B34" s="77"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="77"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="5">
@@ -2334,118 +2335,118 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="71" t="s">
+      <c r="A38" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="71"/>
-      <c r="C38" s="71"/>
-      <c r="D38" s="71"/>
-      <c r="E38" s="71"/>
+      <c r="B38" s="77"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="77"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="70">
+      <c r="A39" s="74">
         <v>4.0999999999999996</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="70">
+      <c r="C39" s="74">
         <v>0.5</v>
       </c>
-      <c r="D39" s="69">
+      <c r="D39" s="75">
         <v>0.25</v>
       </c>
-      <c r="E39" s="67"/>
+      <c r="E39" s="79"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="70"/>
+      <c r="A40" s="74"/>
       <c r="B40" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="70"/>
-      <c r="D40" s="72"/>
-      <c r="E40" s="72"/>
+      <c r="C40" s="74"/>
+      <c r="D40" s="78"/>
+      <c r="E40" s="78"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="70"/>
+      <c r="A41" s="74"/>
       <c r="B41" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="70"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="68"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="70">
+      <c r="A42" s="74">
         <v>4.2</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="70">
+      <c r="C42" s="74">
         <v>1</v>
       </c>
-      <c r="D42" s="65">
+      <c r="D42" s="80">
         <v>0</v>
       </c>
-      <c r="E42" s="67"/>
+      <c r="E42" s="79"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="70"/>
+      <c r="A43" s="74"/>
       <c r="B43" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="70"/>
-      <c r="D43" s="66"/>
-      <c r="E43" s="68"/>
+      <c r="C43" s="74"/>
+      <c r="D43" s="81"/>
+      <c r="E43" s="76"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="70">
+      <c r="A44" s="74">
         <v>4.3</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="70">
+      <c r="C44" s="74">
         <v>0.5</v>
       </c>
-      <c r="D44" s="65">
+      <c r="D44" s="80">
         <v>1</v>
       </c>
-      <c r="E44" s="67"/>
+      <c r="E44" s="79"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="70"/>
+      <c r="A45" s="74"/>
       <c r="B45" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C45" s="70"/>
-      <c r="D45" s="66"/>
-      <c r="E45" s="68"/>
+      <c r="C45" s="74"/>
+      <c r="D45" s="81"/>
+      <c r="E45" s="76"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="70">
+      <c r="A46" s="74">
         <v>4.4000000000000004</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C46" s="70">
+      <c r="C46" s="74">
         <v>0.75</v>
       </c>
-      <c r="D46" s="69">
+      <c r="D46" s="75">
         <v>0.75</v>
       </c>
-      <c r="E46" s="67"/>
+      <c r="E46" s="79"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="70"/>
+      <c r="A47" s="74"/>
       <c r="B47" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C47" s="70"/>
-      <c r="D47" s="68"/>
-      <c r="E47" s="68"/>
+      <c r="C47" s="74"/>
+      <c r="D47" s="76"/>
+      <c r="E47" s="76"/>
       <c r="F47">
         <f>C39*D39+C42*D42+C44*D44+C46*D46</f>
         <v>1.1875</v>
@@ -2471,6 +2472,39 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="A39:A41"/>
@@ -2487,39 +2521,6 @@
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="C29:C32"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="D5:D8"/>
-    <mergeCell ref="E5:E8"/>
-    <mergeCell ref="D9:D14"/>
-    <mergeCell ref="E9:E14"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C42:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
commit hoàn thành đánh giá và duyệt tinraovat(k bít có hoàn thành chưa nữa,tại vs2008 trên máy bị điên,kiểm tra debug k đc)
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="12120" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Phân công" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="61">
   <si>
     <t>STT</t>
   </si>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>Phát tán tin rao vặt</t>
-  </si>
-  <si>
-    <t>Đang dùng phân quyền mặc định</t>
   </si>
   <si>
     <t>Gửi email</t>
@@ -175,9 +172,6 @@
     <t>Đã xong</t>
   </si>
   <si>
-    <t>cơ bản 25%, Làm thêm 75 % là OK</t>
-  </si>
-  <si>
     <t>Mức dộ hoàn thành (%)</t>
   </si>
   <si>
@@ -203,6 +197,12 @@
   </si>
   <si>
     <t>Tích hợp hoàn chỉnh, chưa bỏ trang Tìm Kiếm bên ngoài</t>
+  </si>
+  <si>
+    <t>Đã xong,nhưng do bài chưa host lên localhost nên vẫn phải xài localhost mặc định trên máy</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -376,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -499,9 +499,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -558,6 +555,21 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -855,7 +867,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
@@ -870,28 +884,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="52" t="s">
+      <c r="F1" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="47"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="10">
@@ -907,16 +921,16 @@
       <c r="E2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="45">
+      <c r="F2" s="44">
         <v>1</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="55"/>
+      <c r="I2" s="54"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="10">
@@ -934,10 +948,10 @@
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="59"/>
-      <c r="I3" s="56"/>
+        <v>52</v>
+      </c>
+      <c r="H3" s="58"/>
+      <c r="I3" s="55"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="10">
@@ -955,14 +969,14 @@
       <c r="E4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="45">
+      <c r="F4" s="44">
         <v>1</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="59"/>
-      <c r="I4" s="56"/>
+        <v>53</v>
+      </c>
+      <c r="H4" s="58"/>
+      <c r="I4" s="55"/>
     </row>
     <row r="5" spans="1:9" ht="33">
       <c r="A5" s="10">
@@ -980,14 +994,14 @@
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="45">
+      <c r="F5" s="44">
         <v>1</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="59"/>
-      <c r="I5" s="56"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="55"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="10">
@@ -1005,14 +1019,14 @@
       <c r="E6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="45">
+      <c r="F6" s="44">
         <v>1</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" s="59"/>
-      <c r="I6" s="56"/>
+        <v>54</v>
+      </c>
+      <c r="H6" s="58"/>
+      <c r="I6" s="55"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="10">
@@ -1030,14 +1044,14 @@
       <c r="E7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="45">
+      <c r="F7" s="44">
         <v>1</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" s="59"/>
-      <c r="I7" s="56"/>
+        <v>53</v>
+      </c>
+      <c r="H7" s="58"/>
+      <c r="I7" s="55"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10">
@@ -1055,14 +1069,14 @@
       <c r="E8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="45">
+      <c r="F8" s="44">
         <v>1</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="H8" s="59"/>
-      <c r="I8" s="56"/>
+        <v>55</v>
+      </c>
+      <c r="H8" s="58"/>
+      <c r="I8" s="55"/>
     </row>
     <row r="9" spans="1:9" ht="33">
       <c r="A9" s="10">
@@ -1080,14 +1094,14 @@
       <c r="E9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="45">
+      <c r="F9" s="44">
         <v>1</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="59"/>
-      <c r="I9" s="56"/>
+        <v>58</v>
+      </c>
+      <c r="H9" s="58"/>
+      <c r="I9" s="55"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="14">
@@ -1105,31 +1119,31 @@
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
       <c r="G10" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="59"/>
-      <c r="I10" s="56"/>
+        <v>47</v>
+      </c>
+      <c r="H10" s="58"/>
+      <c r="I10" s="55"/>
     </row>
     <row r="11" spans="1:9" ht="33">
       <c r="A11" s="12">
         <v>10</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="16">
         <v>4.2</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
       <c r="G11" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="59"/>
-      <c r="I11" s="56"/>
+        <v>47</v>
+      </c>
+      <c r="H11" s="58"/>
+      <c r="I11" s="55"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="3">
@@ -1149,12 +1163,12 @@
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="60" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="57"/>
+      <c r="I12" s="56"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3">
@@ -1174,10 +1188,10 @@
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H13" s="60"/>
-      <c r="I13" s="58"/>
+        <v>45</v>
+      </c>
+      <c r="H13" s="59"/>
+      <c r="I13" s="57"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="3">
@@ -1197,8 +1211,8 @@
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="58"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="57"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="3">
@@ -1218,8 +1232,8 @@
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="58"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="57"/>
     </row>
     <row r="16" spans="1:9" ht="33">
       <c r="A16" s="3">
@@ -1239,10 +1253,10 @@
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="60"/>
-      <c r="I16" s="58"/>
+        <v>48</v>
+      </c>
+      <c r="H16" s="59"/>
+      <c r="I16" s="57"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="3">
@@ -1262,17 +1276,17 @@
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H17" s="60"/>
-      <c r="I17" s="58"/>
+        <v>46</v>
+      </c>
+      <c r="H17" s="59"/>
+      <c r="I17" s="57"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="7">
         <v>18</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="7">
         <v>4.3</v>
@@ -1283,10 +1297,10 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H18" s="60"/>
-      <c r="I18" s="58"/>
+        <v>49</v>
+      </c>
+      <c r="H18" s="59"/>
+      <c r="I18" s="57"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="19">
@@ -1306,9 +1320,9 @@
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" s="60" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1330,9 +1344,9 @@
       </c>
       <c r="F20" s="24"/>
       <c r="G20" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" s="61"/>
+        <v>56</v>
+      </c>
+      <c r="H20" s="60"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="21">
@@ -1352,14 +1366,14 @@
       </c>
       <c r="F21" s="25"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="61"/>
+      <c r="H21" s="60"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="21">
         <v>23</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="24"/>
       <c r="D22" s="25" t="s">
@@ -1370,14 +1384,14 @@
       </c>
       <c r="F22" s="25"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="61"/>
+      <c r="H22" s="60"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="24">
         <v>24</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C23" s="24">
         <v>4.4000000000000004</v>
@@ -1389,10 +1403,10 @@
         <v>20</v>
       </c>
       <c r="F23" s="24"/>
-      <c r="G23" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="H23" s="61"/>
+      <c r="G23" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="H23" s="60"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="26">
@@ -1410,9 +1424,13 @@
       <c r="E24" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="53" t="s">
+      <c r="F24" s="65">
+        <v>1</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" s="52" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1432,9 +1450,13 @@
       <c r="E25" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="26"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="53"/>
+      <c r="F25" s="65">
+        <v>1</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" s="52"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="26">
@@ -1454,7 +1476,7 @@
       </c>
       <c r="F26" s="26"/>
       <c r="G26" s="29"/>
-      <c r="H26" s="53"/>
+      <c r="H26" s="52"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="30">
@@ -1472,9 +1494,9 @@
       <c r="E27" s="32"/>
       <c r="F27" s="32"/>
       <c r="G27" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="H27" s="53"/>
+        <v>47</v>
+      </c>
+      <c r="H27" s="52"/>
     </row>
     <row r="28" spans="1:9" ht="33">
       <c r="A28" s="35">
@@ -1492,9 +1514,9 @@
       <c r="E28" s="35"/>
       <c r="F28" s="35"/>
       <c r="G28" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="H28" s="53"/>
+        <v>47</v>
+      </c>
+      <c r="H28" s="52"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="38">
@@ -1512,11 +1534,13 @@
       <c r="E29" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="38"/>
+      <c r="F29" s="63">
+        <v>1</v>
+      </c>
       <c r="G29" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="H29" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="H29" s="53" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1536,9 +1560,13 @@
       <c r="E30" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="38"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="54"/>
+      <c r="F30" s="63">
+        <v>1</v>
+      </c>
+      <c r="G30" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="H30" s="53"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="38">
@@ -1556,18 +1584,20 @@
       <c r="E31" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="F31" s="38"/>
+      <c r="F31" s="63">
+        <v>1</v>
+      </c>
       <c r="G31" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="H31" s="54"/>
+        <v>60</v>
+      </c>
+      <c r="H31" s="53"/>
     </row>
     <row r="32" spans="1:9" ht="49.5">
       <c r="A32" s="34">
         <v>33</v>
       </c>
-      <c r="B32" s="48" t="s">
-        <v>45</v>
+      <c r="B32" s="47" t="s">
+        <v>44</v>
       </c>
       <c r="C32" s="34">
         <v>4.0999999999999996</v>
@@ -1575,32 +1605,36 @@
       <c r="D32" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="H32" s="54"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="61">
+        <v>0.75</v>
+      </c>
+      <c r="H32" s="53"/>
     </row>
     <row r="33" spans="1:8" ht="43.5" customHeight="1">
-      <c r="A33" s="43">
+      <c r="A33" s="42">
         <v>34</v>
       </c>
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="43">
+      <c r="C33" s="42">
         <v>3.3</v>
       </c>
-      <c r="D33" s="44" t="s">
+      <c r="D33" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="H33" s="54"/>
+      <c r="E33" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="64">
+        <v>0.95</v>
+      </c>
+      <c r="G33" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="H33" s="53"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:G31">

</xml_diff>

<commit_message>
chỉnh sửa label hoàn chỉnh
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="62">
   <si>
     <t>STT</t>
   </si>
@@ -373,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -520,6 +520,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -547,38 +580,8 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -876,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -936,10 +939,10 @@
       <c r="G2" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="52"/>
+      <c r="I2" s="63"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="10">
@@ -959,8 +962,8 @@
       <c r="G3" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="56"/>
-      <c r="I3" s="53"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="10">
@@ -984,8 +987,8 @@
       <c r="G4" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="56"/>
-      <c r="I4" s="53"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="64"/>
     </row>
     <row r="5" spans="1:9" ht="33">
       <c r="A5" s="10">
@@ -1009,8 +1012,8 @@
       <c r="G5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="56"/>
-      <c r="I5" s="53"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="64"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="10">
@@ -1034,8 +1037,8 @@
       <c r="G6" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="56"/>
-      <c r="I6" s="53"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="64"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="10">
@@ -1059,8 +1062,8 @@
       <c r="G7" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="56"/>
-      <c r="I7" s="53"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="64"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10">
@@ -1084,8 +1087,8 @@
       <c r="G8" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="56"/>
-      <c r="I8" s="53"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="64"/>
     </row>
     <row r="9" spans="1:9" ht="33">
       <c r="A9" s="10">
@@ -1109,8 +1112,8 @@
       <c r="G9" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="56"/>
-      <c r="I9" s="53"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="64"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="14">
@@ -1130,8 +1133,8 @@
       <c r="G10" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="56"/>
-      <c r="I10" s="53"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="64"/>
     </row>
     <row r="11" spans="1:9" ht="33">
       <c r="A11" s="12">
@@ -1151,8 +1154,8 @@
       <c r="G11" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="56"/>
-      <c r="I11" s="53"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="64"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="3">
@@ -1174,10 +1177,10 @@
       <c r="G12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="57" t="s">
+      <c r="H12" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="54"/>
+      <c r="I12" s="65"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3">
@@ -1199,8 +1202,8 @@
       <c r="G13" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="57"/>
-      <c r="I13" s="55"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="66"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="3">
@@ -1220,8 +1223,8 @@
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="55"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="66"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="3">
@@ -1241,8 +1244,8 @@
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="55"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="66"/>
     </row>
     <row r="16" spans="1:9" ht="33">
       <c r="A16" s="3">
@@ -1264,8 +1267,8 @@
       <c r="G16" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="57"/>
-      <c r="I16" s="55"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="66"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="3">
@@ -1287,8 +1290,8 @@
       <c r="G17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="57"/>
-      <c r="I17" s="55"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="66"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="7">
@@ -1308,8 +1311,8 @@
       <c r="G18" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="57"/>
-      <c r="I18" s="55"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="66"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="19">
@@ -1327,13 +1330,13 @@
       <c r="E19" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="67">
+      <c r="F19" s="58">
         <v>0.98</v>
       </c>
       <c r="G19" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="H19" s="58" t="s">
+      <c r="H19" s="69" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1353,13 +1356,13 @@
       <c r="E20" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="68">
+      <c r="F20" s="59">
         <v>0.98</v>
       </c>
       <c r="G20" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="H20" s="58"/>
+      <c r="H20" s="69"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="21">
@@ -1379,7 +1382,7 @@
       </c>
       <c r="F21" s="25"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="58"/>
+      <c r="H21" s="69"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="21">
@@ -1395,9 +1398,13 @@
       <c r="E22" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="25"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="58"/>
+      <c r="F22" s="70">
+        <v>1</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="69"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="24">
@@ -1415,13 +1422,13 @@
       <c r="E23" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="68">
+      <c r="F23" s="59">
         <v>1</v>
       </c>
       <c r="G23" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="H23" s="58"/>
+      <c r="H23" s="69"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="26">
@@ -1439,13 +1446,13 @@
       <c r="E24" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="63">
+      <c r="F24" s="54">
         <v>1</v>
       </c>
       <c r="G24" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="H24" s="50" t="s">
+      <c r="H24" s="61" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1465,13 +1472,13 @@
       <c r="E25" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="63">
+      <c r="F25" s="54">
         <v>1</v>
       </c>
       <c r="G25" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="H25" s="50"/>
+      <c r="H25" s="61"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="26">
@@ -1489,13 +1496,13 @@
       <c r="E26" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="63">
+      <c r="F26" s="54">
         <v>1</v>
       </c>
       <c r="G26" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="H26" s="50"/>
+      <c r="H26" s="61"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="29">
@@ -1513,13 +1520,13 @@
       <c r="E27" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="64">
+      <c r="F27" s="55">
         <v>1</v>
       </c>
       <c r="G27" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="H27" s="50"/>
+      <c r="H27" s="61"/>
     </row>
     <row r="28" spans="1:9" ht="33">
       <c r="A28" s="34">
@@ -1537,13 +1544,13 @@
       <c r="E28" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="F28" s="65">
+      <c r="F28" s="56">
         <v>1</v>
       </c>
       <c r="G28" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="H28" s="50"/>
+      <c r="H28" s="61"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="37">
@@ -1561,13 +1568,13 @@
       <c r="E29" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="61">
+      <c r="F29" s="52">
         <v>1</v>
       </c>
       <c r="G29" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="H29" s="51" t="s">
+      <c r="H29" s="62" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1587,13 +1594,13 @@
       <c r="E30" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="61">
+      <c r="F30" s="52">
         <v>1</v>
       </c>
       <c r="G30" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="H30" s="51"/>
+      <c r="H30" s="62"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="37">
@@ -1611,13 +1618,13 @@
       <c r="E31" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="F31" s="61">
+      <c r="F31" s="52">
         <v>1</v>
       </c>
       <c r="G31" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="H31" s="51"/>
+      <c r="H31" s="62"/>
     </row>
     <row r="32" spans="1:9" ht="49.5">
       <c r="A32" s="33">
@@ -1632,16 +1639,16 @@
       <c r="D32" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="E32" s="66" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32" s="69">
+      <c r="E32" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="60">
         <v>0.95</v>
       </c>
-      <c r="G32" s="59" t="s">
+      <c r="G32" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="H32" s="51"/>
+      <c r="H32" s="62"/>
     </row>
     <row r="33" spans="1:8" ht="43.5" customHeight="1">
       <c r="A33" s="41">
@@ -1656,16 +1663,16 @@
       <c r="D33" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="F33" s="62">
+      <c r="E33" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="53">
         <v>0.95</v>
       </c>
       <c r="G33" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="H33" s="51"/>
+      <c r="H33" s="62"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:G31">

</xml_diff>

<commit_message>
hoàn thành feature và phát tán tin rao vặt
</commit_message>
<xml_diff>
--- a/Danh sach chuc nang/Features.xlsx
+++ b/Danh sach chuc nang/Features.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="60">
   <si>
     <t>STT</t>
   </si>
@@ -199,13 +199,7 @@
     <t>Tích hợp hoàn chỉnh, chưa bỏ trang Tìm Kiếm bên ngoài</t>
   </si>
   <si>
-    <t>Đã xong,nhưng do bài chưa host lên localhost nên vẫn phải xài localhost mặc định trên máy</t>
-  </si>
-  <si>
     <t>ok</t>
-  </si>
-  <si>
-    <t>k xác định được lấy mã tin rao vặt trong gridview có đúng k</t>
   </si>
 </sst>
 </file>
@@ -553,6 +547,9 @@
     <xf numFmtId="9" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -579,9 +576,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -879,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -939,10 +933,10 @@
       <c r="G2" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="67" t="s">
+      <c r="H2" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="10">
@@ -962,8 +956,8 @@
       <c r="G3" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="67"/>
-      <c r="I3" s="64"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="10">
@@ -987,8 +981,8 @@
       <c r="G4" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="67"/>
-      <c r="I4" s="64"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="65"/>
     </row>
     <row r="5" spans="1:9" ht="33">
       <c r="A5" s="10">
@@ -1012,8 +1006,8 @@
       <c r="G5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="67"/>
-      <c r="I5" s="64"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="65"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="10">
@@ -1037,8 +1031,8 @@
       <c r="G6" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="67"/>
-      <c r="I6" s="64"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="65"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="10">
@@ -1062,8 +1056,8 @@
       <c r="G7" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="67"/>
-      <c r="I7" s="64"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="65"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10">
@@ -1087,8 +1081,8 @@
       <c r="G8" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="67"/>
-      <c r="I8" s="64"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="65"/>
     </row>
     <row r="9" spans="1:9" ht="33">
       <c r="A9" s="10">
@@ -1112,8 +1106,8 @@
       <c r="G9" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="67"/>
-      <c r="I9" s="64"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="65"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="14">
@@ -1133,8 +1127,8 @@
       <c r="G10" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="67"/>
-      <c r="I10" s="64"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="65"/>
     </row>
     <row r="11" spans="1:9" ht="33">
       <c r="A11" s="12">
@@ -1154,8 +1148,8 @@
       <c r="G11" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="67"/>
-      <c r="I11" s="64"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="65"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="3">
@@ -1177,10 +1171,10 @@
       <c r="G12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="68" t="s">
+      <c r="H12" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="65"/>
+      <c r="I12" s="66"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3">
@@ -1202,8 +1196,8 @@
       <c r="G13" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="68"/>
-      <c r="I13" s="66"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="67"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="3">
@@ -1223,8 +1217,8 @@
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="66"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="67"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="3">
@@ -1244,8 +1238,8 @@
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="66"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="67"/>
     </row>
     <row r="16" spans="1:9" ht="33">
       <c r="A16" s="3">
@@ -1267,8 +1261,8 @@
       <c r="G16" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="68"/>
-      <c r="I16" s="66"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="67"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="3">
@@ -1290,8 +1284,8 @@
       <c r="G17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="68"/>
-      <c r="I17" s="66"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="67"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="7">
@@ -1311,8 +1305,8 @@
       <c r="G18" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="68"/>
-      <c r="I18" s="66"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="67"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="19">
@@ -1336,7 +1330,7 @@
       <c r="G19" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="H19" s="69" t="s">
+      <c r="H19" s="70" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1362,7 +1356,7 @@
       <c r="G20" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="H20" s="69"/>
+      <c r="H20" s="70"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="21">
@@ -1382,7 +1376,7 @@
       </c>
       <c r="F21" s="25"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="69"/>
+      <c r="H21" s="70"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="21">
@@ -1398,13 +1392,13 @@
       <c r="E22" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="70">
+      <c r="F22" s="61">
         <v>1</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="H22" s="69"/>
+        <v>59</v>
+      </c>
+      <c r="H22" s="70"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="24">
@@ -1426,9 +1420,9 @@
         <v>1</v>
       </c>
       <c r="G23" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="H23" s="69"/>
+        <v>59</v>
+      </c>
+      <c r="H23" s="70"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="26">
@@ -1450,9 +1444,9 @@
         <v>1</v>
       </c>
       <c r="G24" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="H24" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" s="62" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1476,9 +1470,9 @@
         <v>1</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="H25" s="61"/>
+        <v>59</v>
+      </c>
+      <c r="H25" s="62"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="26">
@@ -1500,9 +1494,9 @@
         <v>1</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="H26" s="61"/>
+        <v>59</v>
+      </c>
+      <c r="H26" s="62"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="29">
@@ -1524,9 +1518,9 @@
         <v>1</v>
       </c>
       <c r="G27" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="H27" s="61"/>
+        <v>59</v>
+      </c>
+      <c r="H27" s="62"/>
     </row>
     <row r="28" spans="1:9" ht="33">
       <c r="A28" s="34">
@@ -1548,9 +1542,9 @@
         <v>1</v>
       </c>
       <c r="G28" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="H28" s="61"/>
+        <v>59</v>
+      </c>
+      <c r="H28" s="62"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="37">
@@ -1572,9 +1566,9 @@
         <v>1</v>
       </c>
       <c r="G29" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="H29" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="H29" s="63" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1598,9 +1592,9 @@
         <v>1</v>
       </c>
       <c r="G30" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="H30" s="62"/>
+        <v>59</v>
+      </c>
+      <c r="H30" s="63"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="37">
@@ -1622,9 +1616,9 @@
         <v>1</v>
       </c>
       <c r="G31" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="H31" s="62"/>
+        <v>59</v>
+      </c>
+      <c r="H31" s="63"/>
     </row>
     <row r="32" spans="1:9" ht="49.5">
       <c r="A32" s="33">
@@ -1643,12 +1637,12 @@
         <v>20</v>
       </c>
       <c r="F32" s="60">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G32" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="H32" s="62"/>
+        <v>59</v>
+      </c>
+      <c r="H32" s="63"/>
     </row>
     <row r="33" spans="1:8" ht="43.5" customHeight="1">
       <c r="A33" s="41">
@@ -1667,12 +1661,12 @@
         <v>20</v>
       </c>
       <c r="F33" s="53">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G33" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="H33" s="62"/>
+      <c r="H33" s="63"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:G31">

</xml_diff>